<commit_message>
Change Controller from Controller to AdminController
</commit_message>
<xml_diff>
--- a/dbShopeeAutomationV2/dbShopeeAutomationV2/Content/Uploads/(NTL) Material Usage Record.xlsx
+++ b/dbShopeeAutomationV2/dbShopeeAutomationV2/Content/Uploads/(NTL) Material Usage Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NTL ERP Demo MP4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F99107-0463-4C27-9C31-308352D314AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C4F030-B244-483A-BE8E-F6808959BAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="568" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier Info" sheetId="1" r:id="rId1"/>
@@ -1565,12 +1565,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1580,9 +1579,43 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1592,62 +1625,29 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1935,12 +1935,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -2139,11 +2139,11 @@
   </sheetPr>
   <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2183,27 +2183,27 @@
       </c>
     </row>
     <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="100" t="s">
+      <c r="D3" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="102" t="s">
+      <c r="E3" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="103" t="s">
+      <c r="F3" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="104"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="106" t="s">
+      <c r="G3" s="103"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="105" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="107" t="s">
@@ -2250,11 +2250,11 @@
       <c r="AE3" s="13"/>
     </row>
     <row r="4" spans="1:31" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="101"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
+      <c r="A4" s="106"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
       <c r="F4" s="15" t="s">
         <v>42</v>
       </c>
@@ -2264,16 +2264,16 @@
       <c r="H4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="101"/>
-      <c r="N4" s="101"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="101"/>
-      <c r="Q4" s="101"/>
-      <c r="R4" s="101"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="106"/>
+      <c r="N4" s="106"/>
+      <c r="O4" s="106"/>
+      <c r="P4" s="106"/>
+      <c r="Q4" s="106"/>
+      <c r="R4" s="106"/>
       <c r="S4" s="14" t="s">
         <v>45</v>
       </c>
@@ -2306,7 +2306,7 @@
       <c r="E5" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="131">
+      <c r="F5" s="101">
         <v>44456</v>
       </c>
       <c r="G5" s="19" t="s">
@@ -2373,7 +2373,7 @@
       <c r="E6" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="131">
+      <c r="F6" s="101">
         <v>44456</v>
       </c>
       <c r="G6" s="19" t="s">
@@ -2440,7 +2440,7 @@
       <c r="E7" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="131">
+      <c r="F7" s="101">
         <v>44456</v>
       </c>
       <c r="G7" s="19" t="s">
@@ -2503,7 +2503,7 @@
       <c r="E8" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="131">
+      <c r="F8" s="101">
         <v>44456</v>
       </c>
       <c r="G8" s="19" t="s">
@@ -2570,7 +2570,7 @@
       <c r="E9" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="130">
+      <c r="F9" s="100">
         <v>44467</v>
       </c>
       <c r="G9" s="31" t="s">
@@ -2644,7 +2644,7 @@
       <c r="E10" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="130">
+      <c r="F10" s="100">
         <v>44522</v>
       </c>
       <c r="G10" s="37" t="s">
@@ -3066,6 +3066,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="Q3:Q4"/>
@@ -3077,11 +3082,6 @@
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="I5:I24">
@@ -3117,11 +3117,11 @@
   </sheetPr>
   <dimension ref="A1:Q1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="9" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3143,7 +3143,7 @@
     <col min="17" max="17" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>101</v>
       </c>
@@ -3163,7 +3163,7 @@
       <c r="O1" s="46"/>
       <c r="P1" s="47"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F2" s="48"/>
       <c r="H2" s="48"/>
       <c r="I2" s="48"/>
@@ -3174,22 +3174,22 @@
       <c r="N2" s="36"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="108" t="s">
+    <row r="3" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="121" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="121" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="109" t="s">
+      <c r="D3" s="122" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="105"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="104"/>
       <c r="H3" s="50"/>
       <c r="I3" s="51" t="s">
         <v>105</v>
@@ -3199,17 +3199,17 @@
       <c r="L3" s="52"/>
       <c r="M3" s="52"/>
       <c r="N3" s="52"/>
-      <c r="O3" s="110" t="s">
+      <c r="O3" s="123" t="s">
         <v>106</v>
       </c>
-      <c r="P3" s="111" t="s">
+      <c r="P3" s="115" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="101"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
+    <row r="4" spans="1:17" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="106"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
       <c r="D4" s="53" t="s">
         <v>44</v>
       </c>
@@ -3243,17 +3243,17 @@
       <c r="N4" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="O4" s="101"/>
-      <c r="P4" s="101"/>
+      <c r="O4" s="106"/>
+      <c r="P4" s="106"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="112">
+      <c r="B5" s="116">
         <v>44470</v>
       </c>
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="113" t="s">
         <v>118</v>
       </c>
       <c r="D5" s="56" t="str">
@@ -3266,7 +3266,7 @@
       <c r="F5" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="115">
+      <c r="G5" s="110">
         <v>0.92</v>
       </c>
       <c r="H5" s="59" t="str">
@@ -3295,7 +3295,7 @@
       <c r="O5" s="63">
         <v>0</v>
       </c>
-      <c r="P5" s="114" t="s">
+      <c r="P5" s="117" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3303,8 +3303,8 @@
       <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="113"/>
-      <c r="C6" s="113"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
       <c r="D6" s="56" t="str">
         <f>'Raw Material Tracking Info'!H5</f>
         <v>A01</v>
@@ -3315,7 +3315,7 @@
       <c r="F6" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="113"/>
+      <c r="G6" s="111"/>
       <c r="H6" s="64" t="str">
         <f t="shared" si="0"/>
         <v>MYV11G-PTRL-VA001-A01</v>
@@ -3342,14 +3342,14 @@
       <c r="O6" s="63">
         <v>0</v>
       </c>
-      <c r="P6" s="113"/>
+      <c r="P6" s="111"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
       <c r="D7" s="56" t="str">
         <f>'Raw Material Tracking Info'!H5</f>
         <v>A01</v>
@@ -3360,7 +3360,7 @@
       <c r="F7" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="101"/>
+      <c r="G7" s="106"/>
       <c r="H7" s="64" t="str">
         <f t="shared" si="0"/>
         <v>MYV18G-PTRL-VA001-A01</v>
@@ -3386,16 +3386,16 @@
       <c r="O7" s="63">
         <v>0</v>
       </c>
-      <c r="P7" s="101"/>
+      <c r="P7" s="106"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="120">
+      <c r="B8" s="112">
         <v>44470</v>
       </c>
-      <c r="C8" s="119" t="s">
+      <c r="C8" s="113" t="s">
         <v>118</v>
       </c>
       <c r="D8" s="57" t="s">
@@ -3407,7 +3407,7 @@
       <c r="F8" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="115">
+      <c r="G8" s="110">
         <v>3.9</v>
       </c>
       <c r="H8" s="64" t="str">
@@ -3446,8 +3446,8 @@
       <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="113"/>
-      <c r="C9" s="113"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="111"/>
       <c r="D9" s="57" t="s">
         <v>51</v>
       </c>
@@ -3457,7 +3457,7 @@
       <c r="F9" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="113"/>
+      <c r="G9" s="111"/>
       <c r="H9" s="64" t="str">
         <f t="shared" si="1"/>
         <v>STR-250-VA001-A01</v>
@@ -3494,8 +3494,8 @@
       <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" s="113"/>
-      <c r="C10" s="113"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="57" t="s">
         <v>51</v>
       </c>
@@ -3505,7 +3505,7 @@
       <c r="F10" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="113"/>
+      <c r="G10" s="111"/>
       <c r="H10" s="64" t="str">
         <f t="shared" si="1"/>
         <v>AXA14G-SMRD-VA001-A01</v>
@@ -3542,8 +3542,8 @@
       <c r="A11" s="6">
         <v>7</v>
       </c>
-      <c r="B11" s="113"/>
-      <c r="C11" s="113"/>
+      <c r="B11" s="111"/>
+      <c r="C11" s="111"/>
       <c r="D11" s="57" t="s">
         <v>51</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="F11" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="113"/>
+      <c r="G11" s="111"/>
       <c r="H11" s="64" t="str">
         <f t="shared" si="1"/>
         <v>AXA14G-SMRP-VA001-A01</v>
@@ -3590,8 +3590,8 @@
       <c r="A12" s="6">
         <v>8</v>
       </c>
-      <c r="B12" s="113"/>
-      <c r="C12" s="113"/>
+      <c r="B12" s="111"/>
+      <c r="C12" s="111"/>
       <c r="D12" s="57" t="s">
         <v>51</v>
       </c>
@@ -3601,7 +3601,7 @@
       <c r="F12" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="113"/>
+      <c r="G12" s="111"/>
       <c r="H12" s="64" t="str">
         <f t="shared" si="1"/>
         <v>AXA14G-PTRL-VA001-A01</v>
@@ -3634,8 +3634,8 @@
       <c r="A13" s="6">
         <v>9</v>
       </c>
-      <c r="B13" s="113"/>
-      <c r="C13" s="113"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
       <c r="D13" s="57" t="s">
         <v>51</v>
       </c>
@@ -3645,7 +3645,7 @@
       <c r="F13" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="113"/>
+      <c r="G13" s="111"/>
       <c r="H13" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV05G-SMRD-VA001-A01</v>
@@ -3678,8 +3678,8 @@
       <c r="A14" s="6">
         <v>10</v>
       </c>
-      <c r="B14" s="113"/>
-      <c r="C14" s="113"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="111"/>
       <c r="D14" s="57" t="s">
         <v>51</v>
       </c>
@@ -3689,7 +3689,7 @@
       <c r="F14" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="113"/>
+      <c r="G14" s="111"/>
       <c r="H14" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV05G-SMRP-VA001-A01</v>
@@ -3722,8 +3722,8 @@
       <c r="A15" s="6">
         <v>11</v>
       </c>
-      <c r="B15" s="113"/>
-      <c r="C15" s="113"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="57" t="s">
         <v>51</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="F15" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="113"/>
+      <c r="G15" s="111"/>
       <c r="H15" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MYV05G-PTRL-VA001-A01</v>
@@ -3766,8 +3766,8 @@
       <c r="A16" s="6">
         <v>12</v>
       </c>
-      <c r="B16" s="113"/>
-      <c r="C16" s="113"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="111"/>
       <c r="D16" s="57" t="s">
         <v>51</v>
       </c>
@@ -3777,7 +3777,7 @@
       <c r="F16" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="113"/>
+      <c r="G16" s="111"/>
       <c r="H16" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV11G-SMRD-VA001-A01</v>
@@ -3810,8 +3810,8 @@
       <c r="A17" s="6">
         <v>13</v>
       </c>
-      <c r="B17" s="113"/>
-      <c r="C17" s="113"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="111"/>
       <c r="D17" s="57" t="s">
         <v>51</v>
       </c>
@@ -3821,7 +3821,7 @@
       <c r="F17" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="113"/>
+      <c r="G17" s="111"/>
       <c r="H17" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV11G-SMRP-VA001-A01</v>
@@ -3854,8 +3854,8 @@
       <c r="A18" s="6">
         <v>14</v>
       </c>
-      <c r="B18" s="113"/>
-      <c r="C18" s="113"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="111"/>
       <c r="D18" s="57" t="s">
         <v>51</v>
       </c>
@@ -3865,7 +3865,7 @@
       <c r="F18" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="113"/>
+      <c r="G18" s="111"/>
       <c r="H18" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV11G-PTRL-VA001-A01</v>
@@ -3898,8 +3898,8 @@
       <c r="A19" s="6">
         <v>15</v>
       </c>
-      <c r="B19" s="113"/>
-      <c r="C19" s="113"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="111"/>
       <c r="D19" s="57" t="s">
         <v>51</v>
       </c>
@@ -3909,7 +3909,7 @@
       <c r="F19" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="113"/>
+      <c r="G19" s="111"/>
       <c r="H19" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV18G-SMRD-VA001-A01</v>
@@ -3942,8 +3942,8 @@
       <c r="A20" s="6">
         <v>16</v>
       </c>
-      <c r="B20" s="113"/>
-      <c r="C20" s="113"/>
+      <c r="B20" s="111"/>
+      <c r="C20" s="111"/>
       <c r="D20" s="57" t="s">
         <v>51</v>
       </c>
@@ -3953,7 +3953,7 @@
       <c r="F20" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="113"/>
+      <c r="G20" s="111"/>
       <c r="H20" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV18G-SMRP-VA001-A01</v>
@@ -3986,8 +3986,8 @@
       <c r="A21" s="6">
         <v>17</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="101"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="106"/>
       <c r="D21" s="57" t="s">
         <v>51</v>
       </c>
@@ -3997,7 +3997,7 @@
       <c r="F21" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G21" s="101"/>
+      <c r="G21" s="106"/>
       <c r="H21" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV18G-PTRL-VA001-A01</v>
@@ -4030,10 +4030,10 @@
       <c r="A22" s="6">
         <v>18</v>
       </c>
-      <c r="B22" s="120">
+      <c r="B22" s="112">
         <v>44470</v>
       </c>
-      <c r="C22" s="119" t="s">
+      <c r="C22" s="113" t="s">
         <v>118</v>
       </c>
       <c r="D22" s="57" t="s">
@@ -4045,7 +4045,7 @@
       <c r="F22" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="115">
+      <c r="G22" s="110">
         <v>2.6</v>
       </c>
       <c r="H22" s="64" t="str">
@@ -4074,7 +4074,7 @@
       <c r="O22" s="63">
         <v>0</v>
       </c>
-      <c r="P22" s="116" t="s">
+      <c r="P22" s="118" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4082,8 +4082,8 @@
       <c r="A23" s="6">
         <v>19</v>
       </c>
-      <c r="B23" s="113"/>
-      <c r="C23" s="113"/>
+      <c r="B23" s="111"/>
+      <c r="C23" s="111"/>
       <c r="D23" s="57" t="s">
         <v>58</v>
       </c>
@@ -4093,7 +4093,7 @@
       <c r="F23" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="113"/>
+      <c r="G23" s="111"/>
       <c r="H23" s="64" t="str">
         <f t="shared" si="7"/>
         <v>STR-250-VA005-A02</v>
@@ -4120,14 +4120,14 @@
       <c r="O23" s="63">
         <v>0</v>
       </c>
-      <c r="P23" s="117"/>
+      <c r="P23" s="119"/>
     </row>
     <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>20</v>
       </c>
-      <c r="B24" s="113"/>
-      <c r="C24" s="113"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="111"/>
       <c r="D24" s="57" t="s">
         <v>58</v>
       </c>
@@ -4137,7 +4137,7 @@
       <c r="F24" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="113"/>
+      <c r="G24" s="111"/>
       <c r="H24" s="64" t="str">
         <f t="shared" si="7"/>
         <v>AXA14G-SMRD-VA005-A02</v>
@@ -4164,14 +4164,14 @@
       <c r="O24" s="63">
         <v>0</v>
       </c>
-      <c r="P24" s="117"/>
+      <c r="P24" s="119"/>
     </row>
     <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>21</v>
       </c>
-      <c r="B25" s="113"/>
-      <c r="C25" s="113"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="111"/>
       <c r="D25" s="57" t="s">
         <v>58</v>
       </c>
@@ -4181,7 +4181,7 @@
       <c r="F25" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="113"/>
+      <c r="G25" s="111"/>
       <c r="H25" s="64" t="str">
         <f t="shared" si="7"/>
         <v>AXA14G-SMRP-VA005-A02</v>
@@ -4208,14 +4208,14 @@
       <c r="O25" s="63">
         <v>0</v>
       </c>
-      <c r="P25" s="117"/>
+      <c r="P25" s="119"/>
     </row>
     <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>22</v>
       </c>
-      <c r="B26" s="113"/>
-      <c r="C26" s="113"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="111"/>
       <c r="D26" s="57" t="s">
         <v>58</v>
       </c>
@@ -4225,7 +4225,7 @@
       <c r="F26" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="113"/>
+      <c r="G26" s="111"/>
       <c r="H26" s="64" t="str">
         <f t="shared" si="7"/>
         <v>AXA14G-PTRL-VA005-A02</v>
@@ -4252,14 +4252,14 @@
       <c r="O26" s="63">
         <v>0</v>
       </c>
-      <c r="P26" s="117"/>
+      <c r="P26" s="119"/>
     </row>
     <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>23</v>
       </c>
-      <c r="B27" s="113"/>
-      <c r="C27" s="113"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
       <c r="D27" s="57" t="s">
         <v>58</v>
       </c>
@@ -4269,7 +4269,7 @@
       <c r="F27" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="113"/>
+      <c r="G27" s="111"/>
       <c r="H27" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV05G-SMRD-VA005-A02</v>
@@ -4296,14 +4296,14 @@
       <c r="O27" s="63">
         <v>0</v>
       </c>
-      <c r="P27" s="117"/>
+      <c r="P27" s="119"/>
     </row>
     <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>24</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="113"/>
+      <c r="B28" s="111"/>
+      <c r="C28" s="111"/>
       <c r="D28" s="57" t="s">
         <v>58</v>
       </c>
@@ -4313,7 +4313,7 @@
       <c r="F28" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="113"/>
+      <c r="G28" s="111"/>
       <c r="H28" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV05G-SMRP-VA005-A02</v>
@@ -4340,14 +4340,14 @@
       <c r="O28" s="63">
         <v>0</v>
       </c>
-      <c r="P28" s="117"/>
+      <c r="P28" s="119"/>
     </row>
     <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>25</v>
       </c>
-      <c r="B29" s="113"/>
-      <c r="C29" s="113"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="111"/>
       <c r="D29" s="57" t="s">
         <v>58</v>
       </c>
@@ -4357,7 +4357,7 @@
       <c r="F29" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G29" s="113"/>
+      <c r="G29" s="111"/>
       <c r="H29" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV05G-PTRL-VA005-A02</v>
@@ -4384,14 +4384,14 @@
       <c r="O29" s="63">
         <v>0</v>
       </c>
-      <c r="P29" s="117"/>
+      <c r="P29" s="119"/>
     </row>
     <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>26</v>
       </c>
-      <c r="B30" s="113"/>
-      <c r="C30" s="113"/>
+      <c r="B30" s="111"/>
+      <c r="C30" s="111"/>
       <c r="D30" s="57" t="s">
         <v>58</v>
       </c>
@@ -4401,7 +4401,7 @@
       <c r="F30" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="113"/>
+      <c r="G30" s="111"/>
       <c r="H30" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV11G-SMRD-VA005-A02</v>
@@ -4428,14 +4428,14 @@
       <c r="O30" s="63">
         <v>0</v>
       </c>
-      <c r="P30" s="117"/>
+      <c r="P30" s="119"/>
     </row>
     <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>27</v>
       </c>
-      <c r="B31" s="113"/>
-      <c r="C31" s="113"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="111"/>
       <c r="D31" s="57" t="s">
         <v>58</v>
       </c>
@@ -4445,7 +4445,7 @@
       <c r="F31" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G31" s="113"/>
+      <c r="G31" s="111"/>
       <c r="H31" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV11G-SMRP-VA005-A02</v>
@@ -4472,14 +4472,14 @@
       <c r="O31" s="63">
         <v>0</v>
       </c>
-      <c r="P31" s="117"/>
+      <c r="P31" s="119"/>
     </row>
     <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>28</v>
       </c>
-      <c r="B32" s="113"/>
-      <c r="C32" s="113"/>
+      <c r="B32" s="111"/>
+      <c r="C32" s="111"/>
       <c r="D32" s="57" t="s">
         <v>58</v>
       </c>
@@ -4489,7 +4489,7 @@
       <c r="F32" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G32" s="113"/>
+      <c r="G32" s="111"/>
       <c r="H32" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV11G-PTRL-VA005-A02</v>
@@ -4516,14 +4516,14 @@
       <c r="O32" s="63">
         <v>0</v>
       </c>
-      <c r="P32" s="117"/>
+      <c r="P32" s="119"/>
     </row>
     <row r="33" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>29</v>
       </c>
-      <c r="B33" s="113"/>
-      <c r="C33" s="113"/>
+      <c r="B33" s="111"/>
+      <c r="C33" s="111"/>
       <c r="D33" s="57" t="s">
         <v>58</v>
       </c>
@@ -4533,7 +4533,7 @@
       <c r="F33" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G33" s="113"/>
+      <c r="G33" s="111"/>
       <c r="H33" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV18G-SMRD-VA005-A02</v>
@@ -4560,14 +4560,14 @@
       <c r="O33" s="63">
         <v>0</v>
       </c>
-      <c r="P33" s="117"/>
+      <c r="P33" s="119"/>
     </row>
     <row r="34" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>30</v>
       </c>
-      <c r="B34" s="113"/>
-      <c r="C34" s="113"/>
+      <c r="B34" s="111"/>
+      <c r="C34" s="111"/>
       <c r="D34" s="57" t="s">
         <v>58</v>
       </c>
@@ -4577,7 +4577,7 @@
       <c r="F34" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G34" s="113"/>
+      <c r="G34" s="111"/>
       <c r="H34" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV18G-SMRP-VA005-A02</v>
@@ -4604,14 +4604,14 @@
       <c r="O34" s="63">
         <v>0</v>
       </c>
-      <c r="P34" s="117"/>
+      <c r="P34" s="119"/>
     </row>
     <row r="35" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>31</v>
       </c>
-      <c r="B35" s="101"/>
-      <c r="C35" s="101"/>
+      <c r="B35" s="106"/>
+      <c r="C35" s="106"/>
       <c r="D35" s="57" t="s">
         <v>58</v>
       </c>
@@ -4621,7 +4621,7 @@
       <c r="F35" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="101"/>
+      <c r="G35" s="106"/>
       <c r="H35" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV18G-PTRL-VA005-A02</v>
@@ -4648,16 +4648,16 @@
       <c r="O35" s="63">
         <v>0</v>
       </c>
-      <c r="P35" s="118"/>
+      <c r="P35" s="120"/>
     </row>
     <row r="36" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>32</v>
       </c>
-      <c r="B36" s="120">
+      <c r="B36" s="112">
         <v>44473</v>
       </c>
-      <c r="C36" s="119" t="s">
+      <c r="C36" s="113" t="s">
         <v>118</v>
       </c>
       <c r="D36" s="57" t="s">
@@ -4669,7 +4669,7 @@
       <c r="F36" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="G36" s="115">
+      <c r="G36" s="110">
         <v>0.5</v>
       </c>
       <c r="H36" s="64" t="str">
@@ -4704,8 +4704,8 @@
       <c r="A37" s="6">
         <v>33</v>
       </c>
-      <c r="B37" s="113"/>
-      <c r="C37" s="113"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="111"/>
       <c r="D37" s="57" t="s">
         <v>51</v>
       </c>
@@ -4715,7 +4715,7 @@
       <c r="F37" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="G37" s="113"/>
+      <c r="G37" s="111"/>
       <c r="H37" s="64" t="str">
         <f t="shared" si="8"/>
         <v>MYV18G-SMRD-VA001-A01</v>
@@ -4748,8 +4748,8 @@
       <c r="A38" s="6">
         <v>34</v>
       </c>
-      <c r="B38" s="113"/>
-      <c r="C38" s="113"/>
+      <c r="B38" s="111"/>
+      <c r="C38" s="111"/>
       <c r="D38" s="57" t="s">
         <v>51</v>
       </c>
@@ -4759,7 +4759,7 @@
       <c r="F38" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="113"/>
+      <c r="G38" s="111"/>
       <c r="H38" s="64" t="str">
         <f t="shared" si="8"/>
         <v>AXA14G-PTRL-VA001-A01</v>
@@ -4792,8 +4792,8 @@
       <c r="A39" s="6">
         <v>35</v>
       </c>
-      <c r="B39" s="101"/>
-      <c r="C39" s="101"/>
+      <c r="B39" s="106"/>
+      <c r="C39" s="106"/>
       <c r="D39" s="57" t="s">
         <v>51</v>
       </c>
@@ -4803,7 +4803,7 @@
       <c r="F39" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="G39" s="101"/>
+      <c r="G39" s="106"/>
       <c r="H39" s="64" t="str">
         <f t="shared" si="8"/>
         <v>MYV18G-SMRP-VA001-A01</v>
@@ -4836,10 +4836,10 @@
       <c r="A40" s="6">
         <v>36</v>
       </c>
-      <c r="B40" s="121">
+      <c r="B40" s="114">
         <v>44473</v>
       </c>
-      <c r="C40" s="115" t="s">
+      <c r="C40" s="110" t="s">
         <v>118</v>
       </c>
       <c r="D40" s="74" t="s">
@@ -4851,7 +4851,7 @@
       <c r="F40" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G40" s="115">
+      <c r="G40" s="110">
         <v>2.4700000000000002</v>
       </c>
       <c r="H40" s="76" t="s">
@@ -4885,8 +4885,8 @@
       <c r="A41" s="6">
         <v>37</v>
       </c>
-      <c r="B41" s="113"/>
-      <c r="C41" s="113"/>
+      <c r="B41" s="111"/>
+      <c r="C41" s="111"/>
       <c r="D41" s="74" t="s">
         <v>58</v>
       </c>
@@ -4896,7 +4896,7 @@
       <c r="F41" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G41" s="113"/>
+      <c r="G41" s="111"/>
       <c r="H41" s="78" t="s">
         <v>175</v>
       </c>
@@ -4928,8 +4928,8 @@
       <c r="A42" s="6">
         <v>38</v>
       </c>
-      <c r="B42" s="113"/>
-      <c r="C42" s="113"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="111"/>
       <c r="D42" s="74" t="s">
         <v>58</v>
       </c>
@@ -4939,7 +4939,7 @@
       <c r="F42" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G42" s="113"/>
+      <c r="G42" s="111"/>
       <c r="H42" s="78" t="s">
         <v>176</v>
       </c>
@@ -4971,8 +4971,8 @@
       <c r="A43" s="6">
         <v>39</v>
       </c>
-      <c r="B43" s="113"/>
-      <c r="C43" s="113"/>
+      <c r="B43" s="111"/>
+      <c r="C43" s="111"/>
       <c r="D43" s="74" t="s">
         <v>58</v>
       </c>
@@ -4982,7 +4982,7 @@
       <c r="F43" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G43" s="113"/>
+      <c r="G43" s="111"/>
       <c r="H43" s="80" t="s">
         <v>177</v>
       </c>
@@ -5014,8 +5014,8 @@
       <c r="A44" s="6">
         <v>40</v>
       </c>
-      <c r="B44" s="113"/>
-      <c r="C44" s="113"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="111"/>
       <c r="D44" s="74" t="s">
         <v>58</v>
       </c>
@@ -5025,7 +5025,7 @@
       <c r="F44" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G44" s="113"/>
+      <c r="G44" s="111"/>
       <c r="H44" s="80" t="s">
         <v>178</v>
       </c>
@@ -5057,8 +5057,8 @@
       <c r="A45" s="6">
         <v>41</v>
       </c>
-      <c r="B45" s="113"/>
-      <c r="C45" s="113"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="111"/>
       <c r="D45" s="74" t="s">
         <v>58</v>
       </c>
@@ -5068,7 +5068,7 @@
       <c r="F45" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G45" s="113"/>
+      <c r="G45" s="111"/>
       <c r="H45" s="78" t="s">
         <v>179</v>
       </c>
@@ -5100,8 +5100,8 @@
       <c r="A46" s="6">
         <v>42</v>
       </c>
-      <c r="B46" s="113"/>
-      <c r="C46" s="113"/>
+      <c r="B46" s="111"/>
+      <c r="C46" s="111"/>
       <c r="D46" s="74" t="s">
         <v>58</v>
       </c>
@@ -5111,7 +5111,7 @@
       <c r="F46" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G46" s="113"/>
+      <c r="G46" s="111"/>
       <c r="H46" s="78" t="s">
         <v>180</v>
       </c>
@@ -5143,8 +5143,8 @@
       <c r="A47" s="6">
         <v>43</v>
       </c>
-      <c r="B47" s="113"/>
-      <c r="C47" s="113"/>
+      <c r="B47" s="111"/>
+      <c r="C47" s="111"/>
       <c r="D47" s="74" t="s">
         <v>58</v>
       </c>
@@ -5154,7 +5154,7 @@
       <c r="F47" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G47" s="113"/>
+      <c r="G47" s="111"/>
       <c r="H47" s="78" t="s">
         <v>181</v>
       </c>
@@ -5186,8 +5186,8 @@
       <c r="A48" s="6">
         <v>44</v>
       </c>
-      <c r="B48" s="113"/>
-      <c r="C48" s="113"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="111"/>
       <c r="D48" s="74" t="s">
         <v>58</v>
       </c>
@@ -5197,7 +5197,7 @@
       <c r="F48" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G48" s="113"/>
+      <c r="G48" s="111"/>
       <c r="H48" s="78" t="s">
         <v>182</v>
       </c>
@@ -5229,8 +5229,8 @@
       <c r="A49" s="6">
         <v>45</v>
       </c>
-      <c r="B49" s="113"/>
-      <c r="C49" s="113"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="111"/>
       <c r="D49" s="74" t="s">
         <v>58</v>
       </c>
@@ -5240,7 +5240,7 @@
       <c r="F49" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G49" s="113"/>
+      <c r="G49" s="111"/>
       <c r="H49" s="78" t="s">
         <v>183</v>
       </c>
@@ -5272,8 +5272,8 @@
       <c r="A50" s="6">
         <v>46</v>
       </c>
-      <c r="B50" s="101"/>
-      <c r="C50" s="101"/>
+      <c r="B50" s="106"/>
+      <c r="C50" s="106"/>
       <c r="D50" s="74" t="s">
         <v>58</v>
       </c>
@@ -5283,7 +5283,7 @@
       <c r="F50" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G50" s="101"/>
+      <c r="G50" s="106"/>
       <c r="H50" s="78" t="s">
         <v>184</v>
       </c>
@@ -5315,10 +5315,10 @@
       <c r="A51" s="6">
         <v>47</v>
       </c>
-      <c r="B51" s="121">
+      <c r="B51" s="114">
         <v>44474</v>
       </c>
-      <c r="C51" s="115" t="s">
+      <c r="C51" s="110" t="s">
         <v>118</v>
       </c>
       <c r="D51" s="74" t="s">
@@ -5330,7 +5330,7 @@
       <c r="F51" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G51" s="115">
+      <c r="G51" s="110">
         <v>3.9</v>
       </c>
       <c r="H51" s="64" t="str">
@@ -5365,8 +5365,8 @@
       <c r="A52" s="6">
         <v>48</v>
       </c>
-      <c r="B52" s="113"/>
-      <c r="C52" s="113"/>
+      <c r="B52" s="111"/>
+      <c r="C52" s="111"/>
       <c r="D52" s="74" t="s">
         <v>70</v>
       </c>
@@ -5376,7 +5376,7 @@
       <c r="F52" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G52" s="113"/>
+      <c r="G52" s="111"/>
       <c r="H52" s="64" t="str">
         <f t="shared" si="9"/>
         <v>STR-250-VA012-A04</v>
@@ -5409,8 +5409,8 @@
       <c r="A53" s="6">
         <v>49</v>
       </c>
-      <c r="B53" s="113"/>
-      <c r="C53" s="113"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="111"/>
       <c r="D53" s="74" t="s">
         <v>70</v>
       </c>
@@ -5420,7 +5420,7 @@
       <c r="F53" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G53" s="113"/>
+      <c r="G53" s="111"/>
       <c r="H53" s="64" t="str">
         <f t="shared" si="9"/>
         <v>AXA14G-SMRD-VA012-A04</v>
@@ -5453,8 +5453,8 @@
       <c r="A54" s="6">
         <v>50</v>
       </c>
-      <c r="B54" s="113"/>
-      <c r="C54" s="113"/>
+      <c r="B54" s="111"/>
+      <c r="C54" s="111"/>
       <c r="D54" s="74" t="s">
         <v>70</v>
       </c>
@@ -5464,7 +5464,7 @@
       <c r="F54" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G54" s="113"/>
+      <c r="G54" s="111"/>
       <c r="H54" s="64" t="str">
         <f t="shared" si="9"/>
         <v>AXA14G-SMRP-VA012-A04</v>
@@ -5497,8 +5497,8 @@
       <c r="A55" s="6">
         <v>51</v>
       </c>
-      <c r="B55" s="113"/>
-      <c r="C55" s="113"/>
+      <c r="B55" s="111"/>
+      <c r="C55" s="111"/>
       <c r="D55" s="74" t="s">
         <v>70</v>
       </c>
@@ -5508,7 +5508,7 @@
       <c r="F55" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G55" s="113"/>
+      <c r="G55" s="111"/>
       <c r="H55" s="64" t="str">
         <f t="shared" si="9"/>
         <v>AXA14G-PTRL-VA012-A04</v>
@@ -5541,8 +5541,8 @@
       <c r="A56" s="6">
         <v>52</v>
       </c>
-      <c r="B56" s="113"/>
-      <c r="C56" s="113"/>
+      <c r="B56" s="111"/>
+      <c r="C56" s="111"/>
       <c r="D56" s="74" t="s">
         <v>70</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="F56" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G56" s="113"/>
+      <c r="G56" s="111"/>
       <c r="H56" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV05G-SMRD-VA012-A04</v>
@@ -5585,8 +5585,8 @@
       <c r="A57" s="6">
         <v>53</v>
       </c>
-      <c r="B57" s="113"/>
-      <c r="C57" s="113"/>
+      <c r="B57" s="111"/>
+      <c r="C57" s="111"/>
       <c r="D57" s="74" t="s">
         <v>70</v>
       </c>
@@ -5596,7 +5596,7 @@
       <c r="F57" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G57" s="113"/>
+      <c r="G57" s="111"/>
       <c r="H57" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV05G-SMRP-VA012-A04</v>
@@ -5629,8 +5629,8 @@
       <c r="A58" s="6">
         <v>54</v>
       </c>
-      <c r="B58" s="113"/>
-      <c r="C58" s="113"/>
+      <c r="B58" s="111"/>
+      <c r="C58" s="111"/>
       <c r="D58" s="74" t="s">
         <v>70</v>
       </c>
@@ -5640,7 +5640,7 @@
       <c r="F58" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G58" s="113"/>
+      <c r="G58" s="111"/>
       <c r="H58" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV05G-PTRL-VA012-A04</v>
@@ -5673,8 +5673,8 @@
       <c r="A59" s="6">
         <v>55</v>
       </c>
-      <c r="B59" s="113"/>
-      <c r="C59" s="113"/>
+      <c r="B59" s="111"/>
+      <c r="C59" s="111"/>
       <c r="D59" s="74" t="s">
         <v>70</v>
       </c>
@@ -5684,7 +5684,7 @@
       <c r="F59" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G59" s="113"/>
+      <c r="G59" s="111"/>
       <c r="H59" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV11G-SMRD-VA012-A04</v>
@@ -5717,8 +5717,8 @@
       <c r="A60" s="6">
         <v>56</v>
       </c>
-      <c r="B60" s="113"/>
-      <c r="C60" s="113"/>
+      <c r="B60" s="111"/>
+      <c r="C60" s="111"/>
       <c r="D60" s="74" t="s">
         <v>70</v>
       </c>
@@ -5728,7 +5728,7 @@
       <c r="F60" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G60" s="113"/>
+      <c r="G60" s="111"/>
       <c r="H60" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV11G-SMRP-VA012-A04</v>
@@ -5761,8 +5761,8 @@
       <c r="A61" s="6">
         <v>57</v>
       </c>
-      <c r="B61" s="113"/>
-      <c r="C61" s="113"/>
+      <c r="B61" s="111"/>
+      <c r="C61" s="111"/>
       <c r="D61" s="74" t="s">
         <v>70</v>
       </c>
@@ -5772,7 +5772,7 @@
       <c r="F61" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G61" s="113"/>
+      <c r="G61" s="111"/>
       <c r="H61" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV11G-PTRL-VA012-A04</v>
@@ -5805,8 +5805,8 @@
       <c r="A62" s="6">
         <v>58</v>
       </c>
-      <c r="B62" s="113"/>
-      <c r="C62" s="113"/>
+      <c r="B62" s="111"/>
+      <c r="C62" s="111"/>
       <c r="D62" s="74" t="s">
         <v>70</v>
       </c>
@@ -5816,7 +5816,7 @@
       <c r="F62" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G62" s="113"/>
+      <c r="G62" s="111"/>
       <c r="H62" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV18G-SMRD-VA012-A04</v>
@@ -5849,8 +5849,8 @@
       <c r="A63" s="6">
         <v>59</v>
       </c>
-      <c r="B63" s="113"/>
-      <c r="C63" s="113"/>
+      <c r="B63" s="111"/>
+      <c r="C63" s="111"/>
       <c r="D63" s="74" t="s">
         <v>70</v>
       </c>
@@ -5860,7 +5860,7 @@
       <c r="F63" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G63" s="113"/>
+      <c r="G63" s="111"/>
       <c r="H63" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV18G-SMRP-VA012-A04</v>
@@ -5893,8 +5893,8 @@
       <c r="A64" s="6">
         <v>60</v>
       </c>
-      <c r="B64" s="101"/>
-      <c r="C64" s="101"/>
+      <c r="B64" s="106"/>
+      <c r="C64" s="106"/>
       <c r="D64" s="74" t="s">
         <v>70</v>
       </c>
@@ -5904,7 +5904,7 @@
       <c r="F64" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G64" s="101"/>
+      <c r="G64" s="106"/>
       <c r="H64" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV18G-PTRL-VA012-A04</v>
@@ -17126,15 +17126,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="G40:G50"/>
-    <mergeCell ref="G51:G64"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="G36:G39"/>
-    <mergeCell ref="B40:B50"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="B51:B64"/>
-    <mergeCell ref="C51:C64"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="P5:P7"/>
@@ -17147,11 +17143,15 @@
     <mergeCell ref="G8:G21"/>
     <mergeCell ref="B22:B35"/>
     <mergeCell ref="C22:C35"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="G40:G50"/>
+    <mergeCell ref="G51:G64"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="G36:G39"/>
+    <mergeCell ref="B40:B50"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="B51:B64"/>
+    <mergeCell ref="C51:C64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17169,7 +17169,7 @@
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17185,45 +17185,45 @@
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="93"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="122" t="s">
+    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="130" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="130" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="122" t="s">
+      <c r="C2" s="130" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="122" t="s">
+      <c r="D2" s="130" t="s">
         <v>215</v>
       </c>
-      <c r="E2" s="123" t="s">
+      <c r="E2" s="131" t="s">
         <v>216</v>
       </c>
-      <c r="F2" s="105"/>
-      <c r="G2" s="124" t="s">
+      <c r="F2" s="104"/>
+      <c r="G2" s="128" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="101"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
+    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="106"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="94" t="s">
         <v>217</v>
       </c>
       <c r="F3" s="95" t="s">
         <v>218</v>
       </c>
-      <c r="G3" s="101"/>
+      <c r="G3" s="106"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="96">
         <v>1</v>
       </c>
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="127" t="s">
         <v>219</v>
       </c>
       <c r="C4" s="126" t="s">
@@ -17249,8 +17249,8 @@
       <c r="A5" s="98">
         <v>2</v>
       </c>
-      <c r="B5" s="113"/>
-      <c r="C5" s="113"/>
+      <c r="B5" s="111"/>
+      <c r="C5" s="111"/>
       <c r="D5" s="19" t="s">
         <v>163</v>
       </c>
@@ -17271,8 +17271,8 @@
       <c r="A6" s="98">
         <v>3</v>
       </c>
-      <c r="B6" s="113"/>
-      <c r="C6" s="113"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
       <c r="D6" s="19" t="s">
         <v>221</v>
       </c>
@@ -17293,8 +17293,8 @@
       <c r="A7" s="98">
         <v>4</v>
       </c>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="111"/>
       <c r="D7" s="19" t="s">
         <v>222</v>
       </c>
@@ -17315,8 +17315,8 @@
       <c r="A8" s="98">
         <v>5</v>
       </c>
-      <c r="B8" s="113"/>
-      <c r="C8" s="101"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="19" t="s">
         <v>191</v>
       </c>
@@ -17337,7 +17337,7 @@
       <c r="A9" s="98">
         <v>6</v>
       </c>
-      <c r="B9" s="113"/>
+      <c r="B9" s="111"/>
       <c r="C9" s="126" t="s">
         <v>223</v>
       </c>
@@ -17361,8 +17361,8 @@
       <c r="A10" s="98">
         <v>7</v>
       </c>
-      <c r="B10" s="113"/>
-      <c r="C10" s="113"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="19" t="s">
         <v>164</v>
       </c>
@@ -17383,8 +17383,8 @@
       <c r="A11" s="98">
         <v>8</v>
       </c>
-      <c r="B11" s="113"/>
-      <c r="C11" s="113"/>
+      <c r="B11" s="111"/>
+      <c r="C11" s="111"/>
       <c r="D11" s="19" t="s">
         <v>224</v>
       </c>
@@ -17405,8 +17405,8 @@
       <c r="A12" s="98">
         <v>9</v>
       </c>
-      <c r="B12" s="113"/>
-      <c r="C12" s="113"/>
+      <c r="B12" s="111"/>
+      <c r="C12" s="111"/>
       <c r="D12" s="19" t="s">
         <v>225</v>
       </c>
@@ -17427,8 +17427,8 @@
       <c r="A13" s="98">
         <v>10</v>
       </c>
-      <c r="B13" s="113"/>
-      <c r="C13" s="101"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="106"/>
       <c r="D13" s="19" t="s">
         <v>192</v>
       </c>
@@ -17449,7 +17449,7 @@
       <c r="A14" s="98">
         <v>11</v>
       </c>
-      <c r="B14" s="113"/>
+      <c r="B14" s="111"/>
       <c r="C14" s="126" t="s">
         <v>226</v>
       </c>
@@ -17473,8 +17473,8 @@
       <c r="A15" s="98">
         <v>12</v>
       </c>
-      <c r="B15" s="113"/>
-      <c r="C15" s="113"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="19" t="s">
         <v>165</v>
       </c>
@@ -17495,8 +17495,8 @@
       <c r="A16" s="98">
         <v>13</v>
       </c>
-      <c r="B16" s="113"/>
-      <c r="C16" s="113"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="111"/>
       <c r="D16" s="19" t="s">
         <v>227</v>
       </c>
@@ -17517,8 +17517,8 @@
       <c r="A17" s="98">
         <v>14</v>
       </c>
-      <c r="B17" s="113"/>
-      <c r="C17" s="113"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="111"/>
       <c r="D17" s="19" t="s">
         <v>228</v>
       </c>
@@ -17539,8 +17539,8 @@
       <c r="A18" s="98">
         <v>15</v>
       </c>
-      <c r="B18" s="113"/>
-      <c r="C18" s="101"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="106"/>
       <c r="D18" s="19" t="s">
         <v>193</v>
       </c>
@@ -17561,7 +17561,7 @@
       <c r="A19" s="98">
         <v>16</v>
       </c>
-      <c r="B19" s="113"/>
+      <c r="B19" s="111"/>
       <c r="C19" s="19" t="s">
         <v>229</v>
       </c>
@@ -17585,7 +17585,7 @@
       <c r="A20" s="98">
         <v>17</v>
       </c>
-      <c r="B20" s="113"/>
+      <c r="B20" s="111"/>
       <c r="C20" s="19" t="s">
         <v>231</v>
       </c>
@@ -17609,7 +17609,7 @@
       <c r="A21" s="98">
         <v>18</v>
       </c>
-      <c r="B21" s="113"/>
+      <c r="B21" s="111"/>
       <c r="C21" s="19" t="s">
         <v>233</v>
       </c>
@@ -17633,7 +17633,7 @@
       <c r="A22" s="98">
         <v>19</v>
       </c>
-      <c r="B22" s="101"/>
+      <c r="B22" s="106"/>
       <c r="C22" s="19" t="s">
         <v>235</v>
       </c>
@@ -17657,10 +17657,10 @@
       <c r="A23" s="98">
         <v>20</v>
       </c>
-      <c r="B23" s="125" t="s">
+      <c r="B23" s="127" t="s">
         <v>237</v>
       </c>
-      <c r="C23" s="129" t="s">
+      <c r="C23" s="124" t="s">
         <v>220</v>
       </c>
       <c r="D23" s="99" t="s">
@@ -17683,8 +17683,8 @@
       <c r="A24" s="98">
         <v>21</v>
       </c>
-      <c r="B24" s="113"/>
-      <c r="C24" s="113"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="111"/>
       <c r="D24" s="99" t="s">
         <v>166</v>
       </c>
@@ -17705,8 +17705,8 @@
       <c r="A25" s="98">
         <v>22</v>
       </c>
-      <c r="B25" s="113"/>
-      <c r="C25" s="113"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="111"/>
       <c r="D25" s="99" t="s">
         <v>238</v>
       </c>
@@ -17727,8 +17727,8 @@
       <c r="A26" s="98">
         <v>23</v>
       </c>
-      <c r="B26" s="113"/>
-      <c r="C26" s="113"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="111"/>
       <c r="D26" s="99" t="s">
         <v>239</v>
       </c>
@@ -17749,8 +17749,8 @@
       <c r="A27" s="98">
         <v>24</v>
       </c>
-      <c r="B27" s="113"/>
-      <c r="C27" s="101"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="106"/>
       <c r="D27" s="99" t="s">
         <v>194</v>
       </c>
@@ -17771,8 +17771,8 @@
       <c r="A28" s="98">
         <v>25</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="129" t="s">
+      <c r="B28" s="111"/>
+      <c r="C28" s="124" t="s">
         <v>223</v>
       </c>
       <c r="D28" s="99" t="s">
@@ -17795,8 +17795,8 @@
       <c r="A29" s="98">
         <v>26</v>
       </c>
-      <c r="B29" s="113"/>
-      <c r="C29" s="113"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="111"/>
       <c r="D29" s="99" t="s">
         <v>167</v>
       </c>
@@ -17817,8 +17817,8 @@
       <c r="A30" s="98">
         <v>27</v>
       </c>
-      <c r="B30" s="113"/>
-      <c r="C30" s="113"/>
+      <c r="B30" s="111"/>
+      <c r="C30" s="111"/>
       <c r="D30" s="99" t="s">
         <v>240</v>
       </c>
@@ -17839,8 +17839,8 @@
       <c r="A31" s="98">
         <v>28</v>
       </c>
-      <c r="B31" s="113"/>
-      <c r="C31" s="113"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="111"/>
       <c r="D31" s="99" t="s">
         <v>241</v>
       </c>
@@ -17861,8 +17861,8 @@
       <c r="A32" s="98">
         <v>29</v>
       </c>
-      <c r="B32" s="113"/>
-      <c r="C32" s="101"/>
+      <c r="B32" s="111"/>
+      <c r="C32" s="106"/>
       <c r="D32" s="99" t="s">
         <v>195</v>
       </c>
@@ -17883,8 +17883,8 @@
       <c r="A33" s="98">
         <v>30</v>
       </c>
-      <c r="B33" s="113"/>
-      <c r="C33" s="129" t="s">
+      <c r="B33" s="111"/>
+      <c r="C33" s="124" t="s">
         <v>226</v>
       </c>
       <c r="D33" s="99" t="s">
@@ -17907,8 +17907,8 @@
       <c r="A34" s="98">
         <v>31</v>
       </c>
-      <c r="B34" s="113"/>
-      <c r="C34" s="113"/>
+      <c r="B34" s="111"/>
+      <c r="C34" s="111"/>
       <c r="D34" s="99" t="s">
         <v>168</v>
       </c>
@@ -17929,8 +17929,8 @@
       <c r="A35" s="98">
         <v>32</v>
       </c>
-      <c r="B35" s="113"/>
-      <c r="C35" s="113"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="111"/>
       <c r="D35" s="99" t="s">
         <v>242</v>
       </c>
@@ -17951,8 +17951,8 @@
       <c r="A36" s="98">
         <v>33</v>
       </c>
-      <c r="B36" s="113"/>
-      <c r="C36" s="113"/>
+      <c r="B36" s="111"/>
+      <c r="C36" s="111"/>
       <c r="D36" s="99" t="s">
         <v>243</v>
       </c>
@@ -17973,8 +17973,8 @@
       <c r="A37" s="98">
         <v>34</v>
       </c>
-      <c r="B37" s="113"/>
-      <c r="C37" s="101"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="106"/>
       <c r="D37" s="99" t="s">
         <v>196</v>
       </c>
@@ -17995,7 +17995,7 @@
       <c r="A38" s="98">
         <v>35</v>
       </c>
-      <c r="B38" s="113"/>
+      <c r="B38" s="111"/>
       <c r="C38" s="99" t="s">
         <v>229</v>
       </c>
@@ -18019,7 +18019,7 @@
       <c r="A39" s="98">
         <v>36</v>
       </c>
-      <c r="B39" s="113"/>
+      <c r="B39" s="111"/>
       <c r="C39" s="99" t="s">
         <v>231</v>
       </c>
@@ -18043,7 +18043,7 @@
       <c r="A40" s="98">
         <v>37</v>
       </c>
-      <c r="B40" s="113"/>
+      <c r="B40" s="111"/>
       <c r="C40" s="99" t="s">
         <v>233</v>
       </c>
@@ -18067,7 +18067,7 @@
       <c r="A41" s="98">
         <v>38</v>
       </c>
-      <c r="B41" s="101"/>
+      <c r="B41" s="106"/>
       <c r="C41" s="99" t="s">
         <v>247</v>
       </c>
@@ -18091,10 +18091,10 @@
       <c r="A42" s="98">
         <v>39</v>
       </c>
-      <c r="B42" s="125" t="s">
+      <c r="B42" s="127" t="s">
         <v>249</v>
       </c>
-      <c r="C42" s="129" t="s">
+      <c r="C42" s="124" t="s">
         <v>220</v>
       </c>
       <c r="D42" s="19" t="s">
@@ -18117,8 +18117,8 @@
       <c r="A43" s="98">
         <v>40</v>
       </c>
-      <c r="B43" s="113"/>
-      <c r="C43" s="113"/>
+      <c r="B43" s="111"/>
+      <c r="C43" s="111"/>
       <c r="D43" s="19" t="s">
         <v>169</v>
       </c>
@@ -18139,8 +18139,8 @@
       <c r="A44" s="98">
         <v>41</v>
       </c>
-      <c r="B44" s="113"/>
-      <c r="C44" s="113"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="111"/>
       <c r="D44" s="19" t="s">
         <v>250</v>
       </c>
@@ -18161,8 +18161,8 @@
       <c r="A45" s="98">
         <v>42</v>
       </c>
-      <c r="B45" s="113"/>
-      <c r="C45" s="113"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="111"/>
       <c r="D45" s="19" t="s">
         <v>251</v>
       </c>
@@ -18183,8 +18183,8 @@
       <c r="A46" s="98">
         <v>43</v>
       </c>
-      <c r="B46" s="113"/>
-      <c r="C46" s="101"/>
+      <c r="B46" s="111"/>
+      <c r="C46" s="106"/>
       <c r="D46" s="19" t="s">
         <v>197</v>
       </c>
@@ -18205,8 +18205,8 @@
       <c r="A47" s="98">
         <v>44</v>
       </c>
-      <c r="B47" s="113"/>
-      <c r="C47" s="129" t="s">
+      <c r="B47" s="111"/>
+      <c r="C47" s="124" t="s">
         <v>223</v>
       </c>
       <c r="D47" s="19" t="s">
@@ -18229,8 +18229,8 @@
       <c r="A48" s="98">
         <v>45</v>
       </c>
-      <c r="B48" s="113"/>
-      <c r="C48" s="113"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="111"/>
       <c r="D48" s="19" t="s">
         <v>170</v>
       </c>
@@ -18251,8 +18251,8 @@
       <c r="A49" s="98">
         <v>46</v>
       </c>
-      <c r="B49" s="113"/>
-      <c r="C49" s="113"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="111"/>
       <c r="D49" s="19" t="s">
         <v>252</v>
       </c>
@@ -18273,8 +18273,8 @@
       <c r="A50" s="98">
         <v>47</v>
       </c>
-      <c r="B50" s="113"/>
-      <c r="C50" s="113"/>
+      <c r="B50" s="111"/>
+      <c r="C50" s="111"/>
       <c r="D50" s="19" t="s">
         <v>253</v>
       </c>
@@ -18295,8 +18295,8 @@
       <c r="A51" s="98">
         <v>48</v>
       </c>
-      <c r="B51" s="113"/>
-      <c r="C51" s="101"/>
+      <c r="B51" s="111"/>
+      <c r="C51" s="106"/>
       <c r="D51" s="19" t="s">
         <v>198</v>
       </c>
@@ -18317,8 +18317,8 @@
       <c r="A52" s="98">
         <v>49</v>
       </c>
-      <c r="B52" s="113"/>
-      <c r="C52" s="129" t="s">
+      <c r="B52" s="111"/>
+      <c r="C52" s="124" t="s">
         <v>226</v>
       </c>
       <c r="D52" s="19" t="s">
@@ -18341,8 +18341,8 @@
       <c r="A53" s="98">
         <v>50</v>
       </c>
-      <c r="B53" s="113"/>
-      <c r="C53" s="113"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="111"/>
       <c r="D53" s="19" t="s">
         <v>171</v>
       </c>
@@ -18363,8 +18363,8 @@
       <c r="A54" s="98">
         <v>51</v>
       </c>
-      <c r="B54" s="113"/>
-      <c r="C54" s="113"/>
+      <c r="B54" s="111"/>
+      <c r="C54" s="111"/>
       <c r="D54" s="19" t="s">
         <v>254</v>
       </c>
@@ -18385,8 +18385,8 @@
       <c r="A55" s="98">
         <v>52</v>
       </c>
-      <c r="B55" s="113"/>
-      <c r="C55" s="113"/>
+      <c r="B55" s="111"/>
+      <c r="C55" s="111"/>
       <c r="D55" s="19" t="s">
         <v>255</v>
       </c>
@@ -18407,8 +18407,8 @@
       <c r="A56" s="98">
         <v>53</v>
       </c>
-      <c r="B56" s="113"/>
-      <c r="C56" s="101"/>
+      <c r="B56" s="111"/>
+      <c r="C56" s="106"/>
       <c r="D56" s="19" t="s">
         <v>199</v>
       </c>
@@ -18429,7 +18429,7 @@
       <c r="A57" s="98">
         <v>54</v>
       </c>
-      <c r="B57" s="113"/>
+      <c r="B57" s="111"/>
       <c r="C57" s="99" t="s">
         <v>229</v>
       </c>
@@ -18453,7 +18453,7 @@
       <c r="A58" s="98">
         <v>55</v>
       </c>
-      <c r="B58" s="113"/>
+      <c r="B58" s="111"/>
       <c r="C58" s="99" t="s">
         <v>231</v>
       </c>
@@ -18477,7 +18477,7 @@
       <c r="A59" s="98">
         <v>56</v>
       </c>
-      <c r="B59" s="113"/>
+      <c r="B59" s="111"/>
       <c r="C59" s="99" t="s">
         <v>233</v>
       </c>
@@ -18501,7 +18501,7 @@
       <c r="A60" s="98">
         <v>57</v>
       </c>
-      <c r="B60" s="101"/>
+      <c r="B60" s="106"/>
       <c r="C60" s="99" t="s">
         <v>235</v>
       </c>
@@ -18525,10 +18525,10 @@
       <c r="A61" s="98">
         <v>58</v>
       </c>
-      <c r="B61" s="127" t="s">
+      <c r="B61" s="129" t="s">
         <v>260</v>
       </c>
-      <c r="C61" s="129" t="s">
+      <c r="C61" s="124" t="s">
         <v>220</v>
       </c>
       <c r="D61" s="19" t="s">
@@ -18551,8 +18551,8 @@
       <c r="A62" s="98">
         <v>59</v>
       </c>
-      <c r="B62" s="113"/>
-      <c r="C62" s="113"/>
+      <c r="B62" s="111"/>
+      <c r="C62" s="111"/>
       <c r="D62" s="19" t="s">
         <v>160</v>
       </c>
@@ -18573,8 +18573,8 @@
       <c r="A63" s="98">
         <v>60</v>
       </c>
-      <c r="B63" s="113"/>
-      <c r="C63" s="113"/>
+      <c r="B63" s="111"/>
+      <c r="C63" s="111"/>
       <c r="D63" s="19" t="s">
         <v>261</v>
       </c>
@@ -18595,8 +18595,8 @@
       <c r="A64" s="98">
         <v>61</v>
       </c>
-      <c r="B64" s="113"/>
-      <c r="C64" s="113"/>
+      <c r="B64" s="111"/>
+      <c r="C64" s="111"/>
       <c r="D64" s="19" t="s">
         <v>262</v>
       </c>
@@ -18617,8 +18617,8 @@
       <c r="A65" s="98">
         <v>62</v>
       </c>
-      <c r="B65" s="113"/>
-      <c r="C65" s="101"/>
+      <c r="B65" s="111"/>
+      <c r="C65" s="106"/>
       <c r="D65" s="19" t="s">
         <v>188</v>
       </c>
@@ -18639,8 +18639,8 @@
       <c r="A66" s="98">
         <v>63</v>
       </c>
-      <c r="B66" s="113"/>
-      <c r="C66" s="129" t="s">
+      <c r="B66" s="111"/>
+      <c r="C66" s="124" t="s">
         <v>223</v>
       </c>
       <c r="D66" s="19" t="s">
@@ -18663,8 +18663,8 @@
       <c r="A67" s="98">
         <v>64</v>
       </c>
-      <c r="B67" s="113"/>
-      <c r="C67" s="113"/>
+      <c r="B67" s="111"/>
+      <c r="C67" s="111"/>
       <c r="D67" s="19" t="s">
         <v>161</v>
       </c>
@@ -18685,8 +18685,8 @@
       <c r="A68" s="98">
         <v>65</v>
       </c>
-      <c r="B68" s="113"/>
-      <c r="C68" s="113"/>
+      <c r="B68" s="111"/>
+      <c r="C68" s="111"/>
       <c r="D68" s="19" t="s">
         <v>263</v>
       </c>
@@ -18707,8 +18707,8 @@
       <c r="A69" s="98">
         <v>66</v>
       </c>
-      <c r="B69" s="113"/>
-      <c r="C69" s="113"/>
+      <c r="B69" s="111"/>
+      <c r="C69" s="111"/>
       <c r="D69" s="19" t="s">
         <v>264</v>
       </c>
@@ -18729,8 +18729,8 @@
       <c r="A70" s="98">
         <v>67</v>
       </c>
-      <c r="B70" s="113"/>
-      <c r="C70" s="101"/>
+      <c r="B70" s="111"/>
+      <c r="C70" s="106"/>
       <c r="D70" s="19" t="s">
         <v>189</v>
       </c>
@@ -18751,8 +18751,8 @@
       <c r="A71" s="98">
         <v>68</v>
       </c>
-      <c r="B71" s="113"/>
-      <c r="C71" s="129" t="s">
+      <c r="B71" s="111"/>
+      <c r="C71" s="124" t="s">
         <v>226</v>
       </c>
       <c r="D71" s="19" t="s">
@@ -18775,8 +18775,8 @@
       <c r="A72" s="98">
         <v>69</v>
       </c>
-      <c r="B72" s="113"/>
-      <c r="C72" s="113"/>
+      <c r="B72" s="111"/>
+      <c r="C72" s="111"/>
       <c r="D72" s="19" t="s">
         <v>162</v>
       </c>
@@ -18797,8 +18797,8 @@
       <c r="A73" s="98">
         <v>70</v>
       </c>
-      <c r="B73" s="113"/>
-      <c r="C73" s="113"/>
+      <c r="B73" s="111"/>
+      <c r="C73" s="111"/>
       <c r="D73" s="19" t="s">
         <v>265</v>
       </c>
@@ -18819,8 +18819,8 @@
       <c r="A74" s="98">
         <v>71</v>
       </c>
-      <c r="B74" s="113"/>
-      <c r="C74" s="113"/>
+      <c r="B74" s="111"/>
+      <c r="C74" s="111"/>
       <c r="D74" s="19" t="s">
         <v>266</v>
       </c>
@@ -18841,8 +18841,8 @@
       <c r="A75" s="98">
         <v>72</v>
       </c>
-      <c r="B75" s="113"/>
-      <c r="C75" s="101"/>
+      <c r="B75" s="111"/>
+      <c r="C75" s="106"/>
       <c r="D75" s="19" t="s">
         <v>190</v>
       </c>
@@ -18863,7 +18863,7 @@
       <c r="A76" s="98">
         <v>73</v>
       </c>
-      <c r="B76" s="113"/>
+      <c r="B76" s="111"/>
       <c r="C76" s="99" t="s">
         <v>229</v>
       </c>
@@ -18887,7 +18887,7 @@
       <c r="A77" s="98">
         <v>74</v>
       </c>
-      <c r="B77" s="113"/>
+      <c r="B77" s="111"/>
       <c r="C77" s="99" t="s">
         <v>231</v>
       </c>
@@ -18911,7 +18911,7 @@
       <c r="A78" s="98">
         <v>75</v>
       </c>
-      <c r="B78" s="113"/>
+      <c r="B78" s="111"/>
       <c r="C78" s="99" t="s">
         <v>233</v>
       </c>
@@ -18935,7 +18935,7 @@
       <c r="A79" s="98">
         <v>76</v>
       </c>
-      <c r="B79" s="101"/>
+      <c r="B79" s="106"/>
       <c r="C79" s="99" t="s">
         <v>235</v>
       </c>
@@ -18959,10 +18959,10 @@
       <c r="A80" s="98">
         <v>77</v>
       </c>
-      <c r="B80" s="128" t="s">
+      <c r="B80" s="125" t="s">
         <v>271</v>
       </c>
-      <c r="C80" s="129" t="s">
+      <c r="C80" s="124" t="s">
         <v>130</v>
       </c>
       <c r="D80" s="19" t="s">
@@ -18985,8 +18985,8 @@
       <c r="A81" s="98">
         <v>78</v>
       </c>
-      <c r="B81" s="113"/>
-      <c r="C81" s="113"/>
+      <c r="B81" s="111"/>
+      <c r="C81" s="111"/>
       <c r="D81" s="19" t="s">
         <v>157</v>
       </c>
@@ -19007,8 +19007,8 @@
       <c r="A82" s="98">
         <v>79</v>
       </c>
-      <c r="B82" s="113"/>
-      <c r="C82" s="113"/>
+      <c r="B82" s="111"/>
+      <c r="C82" s="111"/>
       <c r="D82" s="19" t="s">
         <v>272</v>
       </c>
@@ -19029,8 +19029,8 @@
       <c r="A83" s="98">
         <v>80</v>
       </c>
-      <c r="B83" s="113"/>
-      <c r="C83" s="113"/>
+      <c r="B83" s="111"/>
+      <c r="C83" s="111"/>
       <c r="D83" s="19" t="s">
         <v>273</v>
       </c>
@@ -19051,8 +19051,8 @@
       <c r="A84" s="98">
         <v>81</v>
       </c>
-      <c r="B84" s="113"/>
-      <c r="C84" s="101"/>
+      <c r="B84" s="111"/>
+      <c r="C84" s="106"/>
       <c r="D84" s="19" t="s">
         <v>186</v>
       </c>
@@ -19073,8 +19073,8 @@
       <c r="A85" s="98">
         <v>82</v>
       </c>
-      <c r="B85" s="113"/>
-      <c r="C85" s="129" t="s">
+      <c r="B85" s="111"/>
+      <c r="C85" s="124" t="s">
         <v>133</v>
       </c>
       <c r="D85" s="19" t="s">
@@ -19097,8 +19097,8 @@
       <c r="A86" s="98">
         <v>83</v>
       </c>
-      <c r="B86" s="113"/>
-      <c r="C86" s="113"/>
+      <c r="B86" s="111"/>
+      <c r="C86" s="111"/>
       <c r="D86" s="19" t="s">
         <v>159</v>
       </c>
@@ -19119,8 +19119,8 @@
       <c r="A87" s="98">
         <v>84</v>
       </c>
-      <c r="B87" s="113"/>
-      <c r="C87" s="113"/>
+      <c r="B87" s="111"/>
+      <c r="C87" s="111"/>
       <c r="D87" s="19" t="s">
         <v>274</v>
       </c>
@@ -19141,8 +19141,8 @@
       <c r="A88" s="98">
         <v>85</v>
       </c>
-      <c r="B88" s="113"/>
-      <c r="C88" s="113"/>
+      <c r="B88" s="111"/>
+      <c r="C88" s="111"/>
       <c r="D88" s="19" t="s">
         <v>275</v>
       </c>
@@ -19163,8 +19163,8 @@
       <c r="A89" s="98">
         <v>86</v>
       </c>
-      <c r="B89" s="113"/>
-      <c r="C89" s="101"/>
+      <c r="B89" s="111"/>
+      <c r="C89" s="106"/>
       <c r="D89" s="19" t="s">
         <v>187</v>
       </c>
@@ -19185,8 +19185,8 @@
       <c r="A90" s="98">
         <v>87</v>
       </c>
-      <c r="B90" s="113"/>
-      <c r="C90" s="129" t="s">
+      <c r="B90" s="111"/>
+      <c r="C90" s="124" t="s">
         <v>276</v>
       </c>
       <c r="D90" s="19" t="s">
@@ -19209,8 +19209,8 @@
       <c r="A91" s="98">
         <v>88</v>
       </c>
-      <c r="B91" s="113"/>
-      <c r="C91" s="113"/>
+      <c r="B91" s="111"/>
+      <c r="C91" s="111"/>
       <c r="D91" s="19" t="s">
         <v>278</v>
       </c>
@@ -19231,8 +19231,8 @@
       <c r="A92" s="98">
         <v>89</v>
       </c>
-      <c r="B92" s="113"/>
-      <c r="C92" s="113"/>
+      <c r="B92" s="111"/>
+      <c r="C92" s="111"/>
       <c r="D92" s="19" t="s">
         <v>279</v>
       </c>
@@ -19253,8 +19253,8 @@
       <c r="A93" s="98">
         <v>90</v>
       </c>
-      <c r="B93" s="113"/>
-      <c r="C93" s="113"/>
+      <c r="B93" s="111"/>
+      <c r="C93" s="111"/>
       <c r="D93" s="19" t="s">
         <v>280</v>
       </c>
@@ -19275,8 +19275,8 @@
       <c r="A94" s="98">
         <v>91</v>
       </c>
-      <c r="B94" s="113"/>
-      <c r="C94" s="101"/>
+      <c r="B94" s="111"/>
+      <c r="C94" s="106"/>
       <c r="D94" s="19" t="s">
         <v>281</v>
       </c>
@@ -19297,8 +19297,8 @@
       <c r="A95" s="98">
         <v>92</v>
       </c>
-      <c r="B95" s="113"/>
-      <c r="C95" s="129" t="s">
+      <c r="B95" s="111"/>
+      <c r="C95" s="124" t="s">
         <v>282</v>
       </c>
       <c r="D95" s="19" t="s">
@@ -19321,8 +19321,8 @@
       <c r="A96" s="98">
         <v>93</v>
       </c>
-      <c r="B96" s="113"/>
-      <c r="C96" s="113"/>
+      <c r="B96" s="111"/>
+      <c r="C96" s="111"/>
       <c r="D96" s="19" t="s">
         <v>284</v>
       </c>
@@ -19343,8 +19343,8 @@
       <c r="A97" s="98">
         <v>94</v>
       </c>
-      <c r="B97" s="113"/>
-      <c r="C97" s="113"/>
+      <c r="B97" s="111"/>
+      <c r="C97" s="111"/>
       <c r="D97" s="19" t="s">
         <v>285</v>
       </c>
@@ -19365,8 +19365,8 @@
       <c r="A98" s="98">
         <v>95</v>
       </c>
-      <c r="B98" s="113"/>
-      <c r="C98" s="113"/>
+      <c r="B98" s="111"/>
+      <c r="C98" s="111"/>
       <c r="D98" s="19" t="s">
         <v>286</v>
       </c>
@@ -19387,8 +19387,8 @@
       <c r="A99" s="98">
         <v>96</v>
       </c>
-      <c r="B99" s="113"/>
-      <c r="C99" s="101"/>
+      <c r="B99" s="111"/>
+      <c r="C99" s="106"/>
       <c r="D99" s="19" t="s">
         <v>287</v>
       </c>
@@ -19409,8 +19409,8 @@
       <c r="A100" s="98">
         <v>97</v>
       </c>
-      <c r="B100" s="113"/>
-      <c r="C100" s="129" t="s">
+      <c r="B100" s="111"/>
+      <c r="C100" s="124" t="s">
         <v>288</v>
       </c>
       <c r="D100" s="19" t="s">
@@ -19433,8 +19433,8 @@
       <c r="A101" s="98">
         <v>98</v>
       </c>
-      <c r="B101" s="113"/>
-      <c r="C101" s="113"/>
+      <c r="B101" s="111"/>
+      <c r="C101" s="111"/>
       <c r="D101" s="19" t="s">
         <v>290</v>
       </c>
@@ -19455,8 +19455,8 @@
       <c r="A102" s="98">
         <v>99</v>
       </c>
-      <c r="B102" s="113"/>
-      <c r="C102" s="113"/>
+      <c r="B102" s="111"/>
+      <c r="C102" s="111"/>
       <c r="D102" s="19" t="s">
         <v>291</v>
       </c>
@@ -19477,8 +19477,8 @@
       <c r="A103" s="98">
         <v>100</v>
       </c>
-      <c r="B103" s="113"/>
-      <c r="C103" s="113"/>
+      <c r="B103" s="111"/>
+      <c r="C103" s="111"/>
       <c r="D103" s="19" t="s">
         <v>292</v>
       </c>
@@ -19499,8 +19499,8 @@
       <c r="A104" s="98">
         <v>101</v>
       </c>
-      <c r="B104" s="113"/>
-      <c r="C104" s="101"/>
+      <c r="B104" s="111"/>
+      <c r="C104" s="106"/>
       <c r="D104" s="19" t="s">
         <v>293</v>
       </c>
@@ -19521,8 +19521,8 @@
       <c r="A105" s="98">
         <v>102</v>
       </c>
-      <c r="B105" s="113"/>
-      <c r="C105" s="129" t="s">
+      <c r="B105" s="111"/>
+      <c r="C105" s="124" t="s">
         <v>294</v>
       </c>
       <c r="D105" s="19" t="s">
@@ -19545,8 +19545,8 @@
       <c r="A106" s="98">
         <v>103</v>
       </c>
-      <c r="B106" s="113"/>
-      <c r="C106" s="113"/>
+      <c r="B106" s="111"/>
+      <c r="C106" s="111"/>
       <c r="D106" s="19" t="s">
         <v>296</v>
       </c>
@@ -19567,8 +19567,8 @@
       <c r="A107" s="98">
         <v>104</v>
       </c>
-      <c r="B107" s="113"/>
-      <c r="C107" s="113"/>
+      <c r="B107" s="111"/>
+      <c r="C107" s="111"/>
       <c r="D107" s="19" t="s">
         <v>297</v>
       </c>
@@ -19589,8 +19589,8 @@
       <c r="A108" s="98">
         <v>105</v>
       </c>
-      <c r="B108" s="113"/>
-      <c r="C108" s="113"/>
+      <c r="B108" s="111"/>
+      <c r="C108" s="111"/>
       <c r="D108" s="19" t="s">
         <v>298</v>
       </c>
@@ -19611,8 +19611,8 @@
       <c r="A109" s="98">
         <v>106</v>
       </c>
-      <c r="B109" s="113"/>
-      <c r="C109" s="101"/>
+      <c r="B109" s="111"/>
+      <c r="C109" s="106"/>
       <c r="D109" s="19" t="s">
         <v>299</v>
       </c>
@@ -19633,8 +19633,8 @@
       <c r="A110" s="98">
         <v>107</v>
       </c>
-      <c r="B110" s="113"/>
-      <c r="C110" s="129" t="s">
+      <c r="B110" s="111"/>
+      <c r="C110" s="124" t="s">
         <v>300</v>
       </c>
       <c r="D110" s="19" t="s">
@@ -19657,8 +19657,8 @@
       <c r="A111" s="98">
         <v>108</v>
       </c>
-      <c r="B111" s="113"/>
-      <c r="C111" s="113"/>
+      <c r="B111" s="111"/>
+      <c r="C111" s="111"/>
       <c r="D111" s="19" t="s">
         <v>302</v>
       </c>
@@ -19679,8 +19679,8 @@
       <c r="A112" s="98">
         <v>109</v>
       </c>
-      <c r="B112" s="113"/>
-      <c r="C112" s="113"/>
+      <c r="B112" s="111"/>
+      <c r="C112" s="111"/>
       <c r="D112" s="19" t="s">
         <v>303</v>
       </c>
@@ -19701,8 +19701,8 @@
       <c r="A113" s="98">
         <v>110</v>
       </c>
-      <c r="B113" s="113"/>
-      <c r="C113" s="113"/>
+      <c r="B113" s="111"/>
+      <c r="C113" s="111"/>
       <c r="D113" s="19" t="s">
         <v>304</v>
       </c>
@@ -19723,8 +19723,8 @@
       <c r="A114" s="98">
         <v>111</v>
       </c>
-      <c r="B114" s="113"/>
-      <c r="C114" s="101"/>
+      <c r="B114" s="111"/>
+      <c r="C114" s="106"/>
       <c r="D114" s="19" t="s">
         <v>305</v>
       </c>
@@ -19745,8 +19745,8 @@
       <c r="A115" s="98">
         <v>112</v>
       </c>
-      <c r="B115" s="113"/>
-      <c r="C115" s="129" t="s">
+      <c r="B115" s="111"/>
+      <c r="C115" s="124" t="s">
         <v>306</v>
       </c>
       <c r="D115" s="19" t="s">
@@ -19769,8 +19769,8 @@
       <c r="A116" s="98">
         <v>113</v>
       </c>
-      <c r="B116" s="113"/>
-      <c r="C116" s="113"/>
+      <c r="B116" s="111"/>
+      <c r="C116" s="111"/>
       <c r="D116" s="19" t="s">
         <v>308</v>
       </c>
@@ -19791,8 +19791,8 @@
       <c r="A117" s="98">
         <v>114</v>
       </c>
-      <c r="B117" s="113"/>
-      <c r="C117" s="113"/>
+      <c r="B117" s="111"/>
+      <c r="C117" s="111"/>
       <c r="D117" s="19" t="s">
         <v>309</v>
       </c>
@@ -19813,8 +19813,8 @@
       <c r="A118" s="98">
         <v>115</v>
       </c>
-      <c r="B118" s="113"/>
-      <c r="C118" s="113"/>
+      <c r="B118" s="111"/>
+      <c r="C118" s="111"/>
       <c r="D118" s="19" t="s">
         <v>310</v>
       </c>
@@ -19835,8 +19835,8 @@
       <c r="A119" s="98">
         <v>116</v>
       </c>
-      <c r="B119" s="101"/>
-      <c r="C119" s="101"/>
+      <c r="B119" s="106"/>
+      <c r="C119" s="106"/>
       <c r="D119" s="19" t="s">
         <v>311</v>
       </c>
@@ -22498,6 +22498,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B61:B79"/>
+    <mergeCell ref="C61:C65"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="C71:C75"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="C47:C51"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B4:B22"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="B42:B60"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:F2"/>
     <mergeCell ref="C80:C84"/>
     <mergeCell ref="C85:C89"/>
     <mergeCell ref="B80:B119"/>
@@ -22514,21 +22529,6 @@
     <mergeCell ref="C105:C109"/>
     <mergeCell ref="C110:C114"/>
     <mergeCell ref="C115:C119"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="C47:C51"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B4:B22"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="B42:B60"/>
-    <mergeCell ref="B61:B79"/>
-    <mergeCell ref="C61:C65"/>
-    <mergeCell ref="C66:C70"/>
-    <mergeCell ref="C71:C75"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:G119">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">

</xml_diff>

<commit_message>
Completed Upload Production Function
</commit_message>
<xml_diff>
--- a/dbShopeeAutomationV2/dbShopeeAutomationV2/Content/Uploads/(NTL) Material Usage Record.xlsx
+++ b/dbShopeeAutomationV2/dbShopeeAutomationV2/Content/Uploads/(NTL) Material Usage Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NTL ERP Demo MP4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C4F030-B244-483A-BE8E-F6808959BAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41066DAC-25ED-442F-94C9-867EDE526FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="568" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1571,6 +1571,13 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1579,43 +1586,9 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1625,29 +1598,56 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2140,10 +2140,10 @@
   <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="X5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomRight" activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2183,54 +2183,54 @@
       </c>
     </row>
     <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="108" t="s">
+      <c r="D3" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="109" t="s">
+      <c r="E3" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="103"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="105" t="s">
+      <c r="G3" s="106"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="107" t="s">
+      <c r="J3" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="107" t="s">
+      <c r="K3" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="107" t="s">
+      <c r="L3" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="107" t="s">
+      <c r="M3" s="109" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="107" t="s">
+      <c r="N3" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="107" t="s">
+      <c r="O3" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="107" t="s">
+      <c r="P3" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="107" t="s">
+      <c r="Q3" s="109" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="107" t="s">
+      <c r="R3" s="109" t="s">
         <v>40</v>
       </c>
       <c r="S3" s="13"/>
@@ -2250,11 +2250,11 @@
       <c r="AE3" s="13"/>
     </row>
     <row r="4" spans="1:31" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="106"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
+      <c r="A4" s="103"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
       <c r="F4" s="15" t="s">
         <v>42</v>
       </c>
@@ -2264,16 +2264,16 @@
       <c r="H4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="106"/>
-      <c r="L4" s="106"/>
-      <c r="M4" s="106"/>
-      <c r="N4" s="106"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="106"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="103"/>
+      <c r="Q4" s="103"/>
+      <c r="R4" s="103"/>
       <c r="S4" s="14" t="s">
         <v>45</v>
       </c>
@@ -3066,11 +3066,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="Q3:Q4"/>
@@ -3082,6 +3077,11 @@
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="I5:I24">
@@ -3175,21 +3175,21 @@
       <c r="O2" s="36"/>
     </row>
     <row r="3" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="110" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="110" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="122" t="s">
+      <c r="D3" s="111" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="104"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="107"/>
       <c r="H3" s="50"/>
       <c r="I3" s="51" t="s">
         <v>105</v>
@@ -3199,17 +3199,17 @@
       <c r="L3" s="52"/>
       <c r="M3" s="52"/>
       <c r="N3" s="52"/>
-      <c r="O3" s="123" t="s">
+      <c r="O3" s="112" t="s">
         <v>106</v>
       </c>
-      <c r="P3" s="115" t="s">
+      <c r="P3" s="113" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="106"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
+      <c r="A4" s="103"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="103"/>
       <c r="D4" s="53" t="s">
         <v>44</v>
       </c>
@@ -3243,17 +3243,17 @@
       <c r="N4" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="103"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="116">
+      <c r="B5" s="114">
         <v>44470</v>
       </c>
-      <c r="C5" s="113" t="s">
+      <c r="C5" s="121" t="s">
         <v>118</v>
       </c>
       <c r="D5" s="56" t="str">
@@ -3266,7 +3266,7 @@
       <c r="F5" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="110">
+      <c r="G5" s="117">
         <v>0.92</v>
       </c>
       <c r="H5" s="59" t="str">
@@ -3295,7 +3295,7 @@
       <c r="O5" s="63">
         <v>0</v>
       </c>
-      <c r="P5" s="117" t="s">
+      <c r="P5" s="116" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3303,8 +3303,8 @@
       <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="115"/>
       <c r="D6" s="56" t="str">
         <f>'Raw Material Tracking Info'!H5</f>
         <v>A01</v>
@@ -3315,7 +3315,7 @@
       <c r="F6" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="111"/>
+      <c r="G6" s="115"/>
       <c r="H6" s="64" t="str">
         <f t="shared" si="0"/>
         <v>MYV11G-PTRL-VA001-A01</v>
@@ -3342,14 +3342,14 @@
       <c r="O6" s="63">
         <v>0</v>
       </c>
-      <c r="P6" s="111"/>
+      <c r="P6" s="115"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="106"/>
-      <c r="C7" s="106"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="56" t="str">
         <f>'Raw Material Tracking Info'!H5</f>
         <v>A01</v>
@@ -3360,7 +3360,7 @@
       <c r="F7" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="106"/>
+      <c r="G7" s="103"/>
       <c r="H7" s="64" t="str">
         <f t="shared" si="0"/>
         <v>MYV18G-PTRL-VA001-A01</v>
@@ -3386,16 +3386,16 @@
       <c r="O7" s="63">
         <v>0</v>
       </c>
-      <c r="P7" s="106"/>
+      <c r="P7" s="103"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="112">
+      <c r="B8" s="122">
         <v>44470</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="121" t="s">
         <v>118</v>
       </c>
       <c r="D8" s="57" t="s">
@@ -3407,7 +3407,7 @@
       <c r="F8" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="110">
+      <c r="G8" s="117">
         <v>3.9</v>
       </c>
       <c r="H8" s="64" t="str">
@@ -3446,8 +3446,8 @@
       <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="111"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="115"/>
+      <c r="C9" s="115"/>
       <c r="D9" s="57" t="s">
         <v>51</v>
       </c>
@@ -3457,7 +3457,7 @@
       <c r="F9" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="111"/>
+      <c r="G9" s="115"/>
       <c r="H9" s="64" t="str">
         <f t="shared" si="1"/>
         <v>STR-250-VA001-A01</v>
@@ -3494,8 +3494,8 @@
       <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" s="111"/>
-      <c r="C10" s="111"/>
+      <c r="B10" s="115"/>
+      <c r="C10" s="115"/>
       <c r="D10" s="57" t="s">
         <v>51</v>
       </c>
@@ -3505,7 +3505,7 @@
       <c r="F10" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="111"/>
+      <c r="G10" s="115"/>
       <c r="H10" s="64" t="str">
         <f t="shared" si="1"/>
         <v>AXA14G-SMRD-VA001-A01</v>
@@ -3542,8 +3542,8 @@
       <c r="A11" s="6">
         <v>7</v>
       </c>
-      <c r="B11" s="111"/>
-      <c r="C11" s="111"/>
+      <c r="B11" s="115"/>
+      <c r="C11" s="115"/>
       <c r="D11" s="57" t="s">
         <v>51</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="F11" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="111"/>
+      <c r="G11" s="115"/>
       <c r="H11" s="64" t="str">
         <f t="shared" si="1"/>
         <v>AXA14G-SMRP-VA001-A01</v>
@@ -3590,8 +3590,8 @@
       <c r="A12" s="6">
         <v>8</v>
       </c>
-      <c r="B12" s="111"/>
-      <c r="C12" s="111"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="115"/>
       <c r="D12" s="57" t="s">
         <v>51</v>
       </c>
@@ -3601,7 +3601,7 @@
       <c r="F12" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="111"/>
+      <c r="G12" s="115"/>
       <c r="H12" s="64" t="str">
         <f t="shared" si="1"/>
         <v>AXA14G-PTRL-VA001-A01</v>
@@ -3634,8 +3634,8 @@
       <c r="A13" s="6">
         <v>9</v>
       </c>
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
       <c r="D13" s="57" t="s">
         <v>51</v>
       </c>
@@ -3645,7 +3645,7 @@
       <c r="F13" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="111"/>
+      <c r="G13" s="115"/>
       <c r="H13" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV05G-SMRD-VA001-A01</v>
@@ -3678,8 +3678,8 @@
       <c r="A14" s="6">
         <v>10</v>
       </c>
-      <c r="B14" s="111"/>
-      <c r="C14" s="111"/>
+      <c r="B14" s="115"/>
+      <c r="C14" s="115"/>
       <c r="D14" s="57" t="s">
         <v>51</v>
       </c>
@@ -3689,7 +3689,7 @@
       <c r="F14" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="111"/>
+      <c r="G14" s="115"/>
       <c r="H14" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV05G-SMRP-VA001-A01</v>
@@ -3722,8 +3722,8 @@
       <c r="A15" s="6">
         <v>11</v>
       </c>
-      <c r="B15" s="111"/>
-      <c r="C15" s="111"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="115"/>
       <c r="D15" s="57" t="s">
         <v>51</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="F15" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="111"/>
+      <c r="G15" s="115"/>
       <c r="H15" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MYV05G-PTRL-VA001-A01</v>
@@ -3766,8 +3766,8 @@
       <c r="A16" s="6">
         <v>12</v>
       </c>
-      <c r="B16" s="111"/>
-      <c r="C16" s="111"/>
+      <c r="B16" s="115"/>
+      <c r="C16" s="115"/>
       <c r="D16" s="57" t="s">
         <v>51</v>
       </c>
@@ -3777,7 +3777,7 @@
       <c r="F16" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="111"/>
+      <c r="G16" s="115"/>
       <c r="H16" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV11G-SMRD-VA001-A01</v>
@@ -3810,8 +3810,8 @@
       <c r="A17" s="6">
         <v>13</v>
       </c>
-      <c r="B17" s="111"/>
-      <c r="C17" s="111"/>
+      <c r="B17" s="115"/>
+      <c r="C17" s="115"/>
       <c r="D17" s="57" t="s">
         <v>51</v>
       </c>
@@ -3821,7 +3821,7 @@
       <c r="F17" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="111"/>
+      <c r="G17" s="115"/>
       <c r="H17" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV11G-SMRP-VA001-A01</v>
@@ -3854,8 +3854,8 @@
       <c r="A18" s="6">
         <v>14</v>
       </c>
-      <c r="B18" s="111"/>
-      <c r="C18" s="111"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="115"/>
       <c r="D18" s="57" t="s">
         <v>51</v>
       </c>
@@ -3865,7 +3865,7 @@
       <c r="F18" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="111"/>
+      <c r="G18" s="115"/>
       <c r="H18" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV11G-PTRL-VA001-A01</v>
@@ -3898,8 +3898,8 @@
       <c r="A19" s="6">
         <v>15</v>
       </c>
-      <c r="B19" s="111"/>
-      <c r="C19" s="111"/>
+      <c r="B19" s="115"/>
+      <c r="C19" s="115"/>
       <c r="D19" s="57" t="s">
         <v>51</v>
       </c>
@@ -3909,7 +3909,7 @@
       <c r="F19" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="111"/>
+      <c r="G19" s="115"/>
       <c r="H19" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV18G-SMRD-VA001-A01</v>
@@ -3942,8 +3942,8 @@
       <c r="A20" s="6">
         <v>16</v>
       </c>
-      <c r="B20" s="111"/>
-      <c r="C20" s="111"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="115"/>
       <c r="D20" s="57" t="s">
         <v>51</v>
       </c>
@@ -3953,7 +3953,7 @@
       <c r="F20" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="111"/>
+      <c r="G20" s="115"/>
       <c r="H20" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV18G-SMRP-VA001-A01</v>
@@ -3986,8 +3986,8 @@
       <c r="A21" s="6">
         <v>17</v>
       </c>
-      <c r="B21" s="106"/>
-      <c r="C21" s="106"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="103"/>
       <c r="D21" s="57" t="s">
         <v>51</v>
       </c>
@@ -3997,7 +3997,7 @@
       <c r="F21" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G21" s="106"/>
+      <c r="G21" s="103"/>
       <c r="H21" s="64" t="str">
         <f t="shared" si="1"/>
         <v>MYV18G-PTRL-VA001-A01</v>
@@ -4030,10 +4030,10 @@
       <c r="A22" s="6">
         <v>18</v>
       </c>
-      <c r="B22" s="112">
+      <c r="B22" s="122">
         <v>44470</v>
       </c>
-      <c r="C22" s="113" t="s">
+      <c r="C22" s="121" t="s">
         <v>118</v>
       </c>
       <c r="D22" s="57" t="s">
@@ -4045,7 +4045,7 @@
       <c r="F22" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="110">
+      <c r="G22" s="117">
         <v>2.6</v>
       </c>
       <c r="H22" s="64" t="str">
@@ -4082,8 +4082,8 @@
       <c r="A23" s="6">
         <v>19</v>
       </c>
-      <c r="B23" s="111"/>
-      <c r="C23" s="111"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="115"/>
       <c r="D23" s="57" t="s">
         <v>58</v>
       </c>
@@ -4093,7 +4093,7 @@
       <c r="F23" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="111"/>
+      <c r="G23" s="115"/>
       <c r="H23" s="64" t="str">
         <f t="shared" si="7"/>
         <v>STR-250-VA005-A02</v>
@@ -4126,8 +4126,8 @@
       <c r="A24" s="6">
         <v>20</v>
       </c>
-      <c r="B24" s="111"/>
-      <c r="C24" s="111"/>
+      <c r="B24" s="115"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="57" t="s">
         <v>58</v>
       </c>
@@ -4137,7 +4137,7 @@
       <c r="F24" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="111"/>
+      <c r="G24" s="115"/>
       <c r="H24" s="64" t="str">
         <f t="shared" si="7"/>
         <v>AXA14G-SMRD-VA005-A02</v>
@@ -4170,8 +4170,8 @@
       <c r="A25" s="6">
         <v>21</v>
       </c>
-      <c r="B25" s="111"/>
-      <c r="C25" s="111"/>
+      <c r="B25" s="115"/>
+      <c r="C25" s="115"/>
       <c r="D25" s="57" t="s">
         <v>58</v>
       </c>
@@ -4181,7 +4181,7 @@
       <c r="F25" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="111"/>
+      <c r="G25" s="115"/>
       <c r="H25" s="64" t="str">
         <f t="shared" si="7"/>
         <v>AXA14G-SMRP-VA005-A02</v>
@@ -4214,8 +4214,8 @@
       <c r="A26" s="6">
         <v>22</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
+      <c r="B26" s="115"/>
+      <c r="C26" s="115"/>
       <c r="D26" s="57" t="s">
         <v>58</v>
       </c>
@@ -4225,7 +4225,7 @@
       <c r="F26" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="111"/>
+      <c r="G26" s="115"/>
       <c r="H26" s="64" t="str">
         <f t="shared" si="7"/>
         <v>AXA14G-PTRL-VA005-A02</v>
@@ -4258,8 +4258,8 @@
       <c r="A27" s="6">
         <v>23</v>
       </c>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="115"/>
       <c r="D27" s="57" t="s">
         <v>58</v>
       </c>
@@ -4269,7 +4269,7 @@
       <c r="F27" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="111"/>
+      <c r="G27" s="115"/>
       <c r="H27" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV05G-SMRD-VA005-A02</v>
@@ -4302,8 +4302,8 @@
       <c r="A28" s="6">
         <v>24</v>
       </c>
-      <c r="B28" s="111"/>
-      <c r="C28" s="111"/>
+      <c r="B28" s="115"/>
+      <c r="C28" s="115"/>
       <c r="D28" s="57" t="s">
         <v>58</v>
       </c>
@@ -4313,7 +4313,7 @@
       <c r="F28" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="111"/>
+      <c r="G28" s="115"/>
       <c r="H28" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV05G-SMRP-VA005-A02</v>
@@ -4346,8 +4346,8 @@
       <c r="A29" s="6">
         <v>25</v>
       </c>
-      <c r="B29" s="111"/>
-      <c r="C29" s="111"/>
+      <c r="B29" s="115"/>
+      <c r="C29" s="115"/>
       <c r="D29" s="57" t="s">
         <v>58</v>
       </c>
@@ -4357,7 +4357,7 @@
       <c r="F29" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G29" s="111"/>
+      <c r="G29" s="115"/>
       <c r="H29" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV05G-PTRL-VA005-A02</v>
@@ -4390,8 +4390,8 @@
       <c r="A30" s="6">
         <v>26</v>
       </c>
-      <c r="B30" s="111"/>
-      <c r="C30" s="111"/>
+      <c r="B30" s="115"/>
+      <c r="C30" s="115"/>
       <c r="D30" s="57" t="s">
         <v>58</v>
       </c>
@@ -4401,7 +4401,7 @@
       <c r="F30" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="111"/>
+      <c r="G30" s="115"/>
       <c r="H30" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV11G-SMRD-VA005-A02</v>
@@ -4434,8 +4434,8 @@
       <c r="A31" s="6">
         <v>27</v>
       </c>
-      <c r="B31" s="111"/>
-      <c r="C31" s="111"/>
+      <c r="B31" s="115"/>
+      <c r="C31" s="115"/>
       <c r="D31" s="57" t="s">
         <v>58</v>
       </c>
@@ -4445,7 +4445,7 @@
       <c r="F31" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G31" s="111"/>
+      <c r="G31" s="115"/>
       <c r="H31" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV11G-SMRP-VA005-A02</v>
@@ -4478,8 +4478,8 @@
       <c r="A32" s="6">
         <v>28</v>
       </c>
-      <c r="B32" s="111"/>
-      <c r="C32" s="111"/>
+      <c r="B32" s="115"/>
+      <c r="C32" s="115"/>
       <c r="D32" s="57" t="s">
         <v>58</v>
       </c>
@@ -4489,7 +4489,7 @@
       <c r="F32" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G32" s="111"/>
+      <c r="G32" s="115"/>
       <c r="H32" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV11G-PTRL-VA005-A02</v>
@@ -4522,8 +4522,8 @@
       <c r="A33" s="6">
         <v>29</v>
       </c>
-      <c r="B33" s="111"/>
-      <c r="C33" s="111"/>
+      <c r="B33" s="115"/>
+      <c r="C33" s="115"/>
       <c r="D33" s="57" t="s">
         <v>58</v>
       </c>
@@ -4533,7 +4533,7 @@
       <c r="F33" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G33" s="111"/>
+      <c r="G33" s="115"/>
       <c r="H33" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV18G-SMRD-VA005-A02</v>
@@ -4566,8 +4566,8 @@
       <c r="A34" s="6">
         <v>30</v>
       </c>
-      <c r="B34" s="111"/>
-      <c r="C34" s="111"/>
+      <c r="B34" s="115"/>
+      <c r="C34" s="115"/>
       <c r="D34" s="57" t="s">
         <v>58</v>
       </c>
@@ -4577,7 +4577,7 @@
       <c r="F34" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G34" s="111"/>
+      <c r="G34" s="115"/>
       <c r="H34" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV18G-SMRP-VA005-A02</v>
@@ -4610,8 +4610,8 @@
       <c r="A35" s="6">
         <v>31</v>
       </c>
-      <c r="B35" s="106"/>
-      <c r="C35" s="106"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="103"/>
       <c r="D35" s="57" t="s">
         <v>58</v>
       </c>
@@ -4621,7 +4621,7 @@
       <c r="F35" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="106"/>
+      <c r="G35" s="103"/>
       <c r="H35" s="64" t="str">
         <f t="shared" si="7"/>
         <v>MYV18G-PTRL-VA005-A02</v>
@@ -4654,10 +4654,10 @@
       <c r="A36" s="6">
         <v>32</v>
       </c>
-      <c r="B36" s="112">
+      <c r="B36" s="122">
         <v>44473</v>
       </c>
-      <c r="C36" s="113" t="s">
+      <c r="C36" s="121" t="s">
         <v>118</v>
       </c>
       <c r="D36" s="57" t="s">
@@ -4669,7 +4669,7 @@
       <c r="F36" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="G36" s="110">
+      <c r="G36" s="117">
         <v>0.5</v>
       </c>
       <c r="H36" s="64" t="str">
@@ -4704,8 +4704,8 @@
       <c r="A37" s="6">
         <v>33</v>
       </c>
-      <c r="B37" s="111"/>
-      <c r="C37" s="111"/>
+      <c r="B37" s="115"/>
+      <c r="C37" s="115"/>
       <c r="D37" s="57" t="s">
         <v>51</v>
       </c>
@@ -4715,7 +4715,7 @@
       <c r="F37" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="G37" s="111"/>
+      <c r="G37" s="115"/>
       <c r="H37" s="64" t="str">
         <f t="shared" si="8"/>
         <v>MYV18G-SMRD-VA001-A01</v>
@@ -4748,8 +4748,8 @@
       <c r="A38" s="6">
         <v>34</v>
       </c>
-      <c r="B38" s="111"/>
-      <c r="C38" s="111"/>
+      <c r="B38" s="115"/>
+      <c r="C38" s="115"/>
       <c r="D38" s="57" t="s">
         <v>51</v>
       </c>
@@ -4759,7 +4759,7 @@
       <c r="F38" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="111"/>
+      <c r="G38" s="115"/>
       <c r="H38" s="64" t="str">
         <f t="shared" si="8"/>
         <v>AXA14G-PTRL-VA001-A01</v>
@@ -4792,8 +4792,8 @@
       <c r="A39" s="6">
         <v>35</v>
       </c>
-      <c r="B39" s="106"/>
-      <c r="C39" s="106"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="103"/>
       <c r="D39" s="57" t="s">
         <v>51</v>
       </c>
@@ -4803,7 +4803,7 @@
       <c r="F39" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="G39" s="106"/>
+      <c r="G39" s="103"/>
       <c r="H39" s="64" t="str">
         <f t="shared" si="8"/>
         <v>MYV18G-SMRP-VA001-A01</v>
@@ -4836,10 +4836,10 @@
       <c r="A40" s="6">
         <v>36</v>
       </c>
-      <c r="B40" s="114">
+      <c r="B40" s="123">
         <v>44473</v>
       </c>
-      <c r="C40" s="110" t="s">
+      <c r="C40" s="117" t="s">
         <v>118</v>
       </c>
       <c r="D40" s="74" t="s">
@@ -4851,7 +4851,7 @@
       <c r="F40" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G40" s="110">
+      <c r="G40" s="117">
         <v>2.4700000000000002</v>
       </c>
       <c r="H40" s="76" t="s">
@@ -4885,8 +4885,8 @@
       <c r="A41" s="6">
         <v>37</v>
       </c>
-      <c r="B41" s="111"/>
-      <c r="C41" s="111"/>
+      <c r="B41" s="115"/>
+      <c r="C41" s="115"/>
       <c r="D41" s="74" t="s">
         <v>58</v>
       </c>
@@ -4896,7 +4896,7 @@
       <c r="F41" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G41" s="111"/>
+      <c r="G41" s="115"/>
       <c r="H41" s="78" t="s">
         <v>175</v>
       </c>
@@ -4928,8 +4928,8 @@
       <c r="A42" s="6">
         <v>38</v>
       </c>
-      <c r="B42" s="111"/>
-      <c r="C42" s="111"/>
+      <c r="B42" s="115"/>
+      <c r="C42" s="115"/>
       <c r="D42" s="74" t="s">
         <v>58</v>
       </c>
@@ -4939,7 +4939,7 @@
       <c r="F42" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G42" s="111"/>
+      <c r="G42" s="115"/>
       <c r="H42" s="78" t="s">
         <v>176</v>
       </c>
@@ -4971,8 +4971,8 @@
       <c r="A43" s="6">
         <v>39</v>
       </c>
-      <c r="B43" s="111"/>
-      <c r="C43" s="111"/>
+      <c r="B43" s="115"/>
+      <c r="C43" s="115"/>
       <c r="D43" s="74" t="s">
         <v>58</v>
       </c>
@@ -4982,7 +4982,7 @@
       <c r="F43" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G43" s="111"/>
+      <c r="G43" s="115"/>
       <c r="H43" s="80" t="s">
         <v>177</v>
       </c>
@@ -5014,8 +5014,8 @@
       <c r="A44" s="6">
         <v>40</v>
       </c>
-      <c r="B44" s="111"/>
-      <c r="C44" s="111"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="115"/>
       <c r="D44" s="74" t="s">
         <v>58</v>
       </c>
@@ -5025,7 +5025,7 @@
       <c r="F44" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G44" s="111"/>
+      <c r="G44" s="115"/>
       <c r="H44" s="80" t="s">
         <v>178</v>
       </c>
@@ -5057,8 +5057,8 @@
       <c r="A45" s="6">
         <v>41</v>
       </c>
-      <c r="B45" s="111"/>
-      <c r="C45" s="111"/>
+      <c r="B45" s="115"/>
+      <c r="C45" s="115"/>
       <c r="D45" s="74" t="s">
         <v>58</v>
       </c>
@@ -5068,7 +5068,7 @@
       <c r="F45" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G45" s="111"/>
+      <c r="G45" s="115"/>
       <c r="H45" s="78" t="s">
         <v>179</v>
       </c>
@@ -5100,8 +5100,8 @@
       <c r="A46" s="6">
         <v>42</v>
       </c>
-      <c r="B46" s="111"/>
-      <c r="C46" s="111"/>
+      <c r="B46" s="115"/>
+      <c r="C46" s="115"/>
       <c r="D46" s="74" t="s">
         <v>58</v>
       </c>
@@ -5111,7 +5111,7 @@
       <c r="F46" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G46" s="111"/>
+      <c r="G46" s="115"/>
       <c r="H46" s="78" t="s">
         <v>180</v>
       </c>
@@ -5143,8 +5143,8 @@
       <c r="A47" s="6">
         <v>43</v>
       </c>
-      <c r="B47" s="111"/>
-      <c r="C47" s="111"/>
+      <c r="B47" s="115"/>
+      <c r="C47" s="115"/>
       <c r="D47" s="74" t="s">
         <v>58</v>
       </c>
@@ -5154,7 +5154,7 @@
       <c r="F47" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G47" s="111"/>
+      <c r="G47" s="115"/>
       <c r="H47" s="78" t="s">
         <v>181</v>
       </c>
@@ -5186,8 +5186,8 @@
       <c r="A48" s="6">
         <v>44</v>
       </c>
-      <c r="B48" s="111"/>
-      <c r="C48" s="111"/>
+      <c r="B48" s="115"/>
+      <c r="C48" s="115"/>
       <c r="D48" s="74" t="s">
         <v>58</v>
       </c>
@@ -5197,7 +5197,7 @@
       <c r="F48" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G48" s="111"/>
+      <c r="G48" s="115"/>
       <c r="H48" s="78" t="s">
         <v>182</v>
       </c>
@@ -5229,8 +5229,8 @@
       <c r="A49" s="6">
         <v>45</v>
       </c>
-      <c r="B49" s="111"/>
-      <c r="C49" s="111"/>
+      <c r="B49" s="115"/>
+      <c r="C49" s="115"/>
       <c r="D49" s="74" t="s">
         <v>58</v>
       </c>
@@ -5240,7 +5240,7 @@
       <c r="F49" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G49" s="111"/>
+      <c r="G49" s="115"/>
       <c r="H49" s="78" t="s">
         <v>183</v>
       </c>
@@ -5272,8 +5272,8 @@
       <c r="A50" s="6">
         <v>46</v>
       </c>
-      <c r="B50" s="106"/>
-      <c r="C50" s="106"/>
+      <c r="B50" s="103"/>
+      <c r="C50" s="103"/>
       <c r="D50" s="74" t="s">
         <v>58</v>
       </c>
@@ -5283,7 +5283,7 @@
       <c r="F50" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G50" s="106"/>
+      <c r="G50" s="103"/>
       <c r="H50" s="78" t="s">
         <v>184</v>
       </c>
@@ -5315,10 +5315,10 @@
       <c r="A51" s="6">
         <v>47</v>
       </c>
-      <c r="B51" s="114">
+      <c r="B51" s="123">
         <v>44474</v>
       </c>
-      <c r="C51" s="110" t="s">
+      <c r="C51" s="117" t="s">
         <v>118</v>
       </c>
       <c r="D51" s="74" t="s">
@@ -5330,7 +5330,7 @@
       <c r="F51" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G51" s="110">
+      <c r="G51" s="117">
         <v>3.9</v>
       </c>
       <c r="H51" s="64" t="str">
@@ -5365,8 +5365,8 @@
       <c r="A52" s="6">
         <v>48</v>
       </c>
-      <c r="B52" s="111"/>
-      <c r="C52" s="111"/>
+      <c r="B52" s="115"/>
+      <c r="C52" s="115"/>
       <c r="D52" s="74" t="s">
         <v>70</v>
       </c>
@@ -5376,7 +5376,7 @@
       <c r="F52" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G52" s="111"/>
+      <c r="G52" s="115"/>
       <c r="H52" s="64" t="str">
         <f t="shared" si="9"/>
         <v>STR-250-VA012-A04</v>
@@ -5409,8 +5409,8 @@
       <c r="A53" s="6">
         <v>49</v>
       </c>
-      <c r="B53" s="111"/>
-      <c r="C53" s="111"/>
+      <c r="B53" s="115"/>
+      <c r="C53" s="115"/>
       <c r="D53" s="74" t="s">
         <v>70</v>
       </c>
@@ -5420,7 +5420,7 @@
       <c r="F53" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G53" s="111"/>
+      <c r="G53" s="115"/>
       <c r="H53" s="64" t="str">
         <f t="shared" si="9"/>
         <v>AXA14G-SMRD-VA012-A04</v>
@@ -5453,8 +5453,8 @@
       <c r="A54" s="6">
         <v>50</v>
       </c>
-      <c r="B54" s="111"/>
-      <c r="C54" s="111"/>
+      <c r="B54" s="115"/>
+      <c r="C54" s="115"/>
       <c r="D54" s="74" t="s">
         <v>70</v>
       </c>
@@ -5464,7 +5464,7 @@
       <c r="F54" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G54" s="111"/>
+      <c r="G54" s="115"/>
       <c r="H54" s="64" t="str">
         <f t="shared" si="9"/>
         <v>AXA14G-SMRP-VA012-A04</v>
@@ -5497,8 +5497,8 @@
       <c r="A55" s="6">
         <v>51</v>
       </c>
-      <c r="B55" s="111"/>
-      <c r="C55" s="111"/>
+      <c r="B55" s="115"/>
+      <c r="C55" s="115"/>
       <c r="D55" s="74" t="s">
         <v>70</v>
       </c>
@@ -5508,7 +5508,7 @@
       <c r="F55" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G55" s="111"/>
+      <c r="G55" s="115"/>
       <c r="H55" s="64" t="str">
         <f t="shared" si="9"/>
         <v>AXA14G-PTRL-VA012-A04</v>
@@ -5541,8 +5541,8 @@
       <c r="A56" s="6">
         <v>52</v>
       </c>
-      <c r="B56" s="111"/>
-      <c r="C56" s="111"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="115"/>
       <c r="D56" s="74" t="s">
         <v>70</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="F56" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G56" s="111"/>
+      <c r="G56" s="115"/>
       <c r="H56" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV05G-SMRD-VA012-A04</v>
@@ -5585,8 +5585,8 @@
       <c r="A57" s="6">
         <v>53</v>
       </c>
-      <c r="B57" s="111"/>
-      <c r="C57" s="111"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="115"/>
       <c r="D57" s="74" t="s">
         <v>70</v>
       </c>
@@ -5596,7 +5596,7 @@
       <c r="F57" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G57" s="111"/>
+      <c r="G57" s="115"/>
       <c r="H57" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV05G-SMRP-VA012-A04</v>
@@ -5629,8 +5629,8 @@
       <c r="A58" s="6">
         <v>54</v>
       </c>
-      <c r="B58" s="111"/>
-      <c r="C58" s="111"/>
+      <c r="B58" s="115"/>
+      <c r="C58" s="115"/>
       <c r="D58" s="74" t="s">
         <v>70</v>
       </c>
@@ -5640,7 +5640,7 @@
       <c r="F58" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G58" s="111"/>
+      <c r="G58" s="115"/>
       <c r="H58" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV05G-PTRL-VA012-A04</v>
@@ -5673,8 +5673,8 @@
       <c r="A59" s="6">
         <v>55</v>
       </c>
-      <c r="B59" s="111"/>
-      <c r="C59" s="111"/>
+      <c r="B59" s="115"/>
+      <c r="C59" s="115"/>
       <c r="D59" s="74" t="s">
         <v>70</v>
       </c>
@@ -5684,7 +5684,7 @@
       <c r="F59" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G59" s="111"/>
+      <c r="G59" s="115"/>
       <c r="H59" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV11G-SMRD-VA012-A04</v>
@@ -5717,8 +5717,8 @@
       <c r="A60" s="6">
         <v>56</v>
       </c>
-      <c r="B60" s="111"/>
-      <c r="C60" s="111"/>
+      <c r="B60" s="115"/>
+      <c r="C60" s="115"/>
       <c r="D60" s="74" t="s">
         <v>70</v>
       </c>
@@ -5728,7 +5728,7 @@
       <c r="F60" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G60" s="111"/>
+      <c r="G60" s="115"/>
       <c r="H60" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV11G-SMRP-VA012-A04</v>
@@ -5761,8 +5761,8 @@
       <c r="A61" s="6">
         <v>57</v>
       </c>
-      <c r="B61" s="111"/>
-      <c r="C61" s="111"/>
+      <c r="B61" s="115"/>
+      <c r="C61" s="115"/>
       <c r="D61" s="74" t="s">
         <v>70</v>
       </c>
@@ -5772,7 +5772,7 @@
       <c r="F61" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G61" s="111"/>
+      <c r="G61" s="115"/>
       <c r="H61" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV11G-PTRL-VA012-A04</v>
@@ -5805,8 +5805,8 @@
       <c r="A62" s="6">
         <v>58</v>
       </c>
-      <c r="B62" s="111"/>
-      <c r="C62" s="111"/>
+      <c r="B62" s="115"/>
+      <c r="C62" s="115"/>
       <c r="D62" s="74" t="s">
         <v>70</v>
       </c>
@@ -5816,7 +5816,7 @@
       <c r="F62" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G62" s="111"/>
+      <c r="G62" s="115"/>
       <c r="H62" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV18G-SMRD-VA012-A04</v>
@@ -5849,8 +5849,8 @@
       <c r="A63" s="6">
         <v>59</v>
       </c>
-      <c r="B63" s="111"/>
-      <c r="C63" s="111"/>
+      <c r="B63" s="115"/>
+      <c r="C63" s="115"/>
       <c r="D63" s="74" t="s">
         <v>70</v>
       </c>
@@ -5860,7 +5860,7 @@
       <c r="F63" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G63" s="111"/>
+      <c r="G63" s="115"/>
       <c r="H63" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV18G-SMRP-VA012-A04</v>
@@ -5893,8 +5893,8 @@
       <c r="A64" s="6">
         <v>60</v>
       </c>
-      <c r="B64" s="106"/>
-      <c r="C64" s="106"/>
+      <c r="B64" s="103"/>
+      <c r="C64" s="103"/>
       <c r="D64" s="74" t="s">
         <v>70</v>
       </c>
@@ -5904,7 +5904,7 @@
       <c r="F64" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G64" s="106"/>
+      <c r="G64" s="103"/>
       <c r="H64" s="64" t="str">
         <f t="shared" si="9"/>
         <v>MYV18G-PTRL-VA012-A04</v>
@@ -17126,11 +17126,15 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="G40:G50"/>
+    <mergeCell ref="G51:G64"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="G36:G39"/>
+    <mergeCell ref="B40:B50"/>
+    <mergeCell ref="C40:C50"/>
+    <mergeCell ref="B51:B64"/>
+    <mergeCell ref="C51:C64"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="P5:P7"/>
@@ -17143,15 +17147,11 @@
     <mergeCell ref="G8:G21"/>
     <mergeCell ref="B22:B35"/>
     <mergeCell ref="C22:C35"/>
-    <mergeCell ref="G40:G50"/>
-    <mergeCell ref="G51:G64"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="G36:G39"/>
-    <mergeCell ref="B40:B50"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="B51:B64"/>
-    <mergeCell ref="C51:C64"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="O3:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17186,47 +17186,47 @@
       <c r="G1" s="93"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="126" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="126" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="126" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="130" t="s">
+      <c r="D2" s="126" t="s">
         <v>215</v>
       </c>
-      <c r="E2" s="131" t="s">
+      <c r="E2" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="F2" s="104"/>
-      <c r="G2" s="128" t="s">
+      <c r="F2" s="107"/>
+      <c r="G2" s="127" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="106"/>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
+      <c r="A3" s="103"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
       <c r="E3" s="94" t="s">
         <v>217</v>
       </c>
       <c r="F3" s="95" t="s">
         <v>218</v>
       </c>
-      <c r="G3" s="106"/>
+      <c r="G3" s="103"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="96">
         <v>1</v>
       </c>
-      <c r="B4" s="127" t="s">
+      <c r="B4" s="128" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="126" t="s">
+      <c r="C4" s="129" t="s">
         <v>220</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -17249,8 +17249,8 @@
       <c r="A5" s="98">
         <v>2</v>
       </c>
-      <c r="B5" s="111"/>
-      <c r="C5" s="111"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
       <c r="D5" s="19" t="s">
         <v>163</v>
       </c>
@@ -17271,8 +17271,8 @@
       <c r="A6" s="98">
         <v>3</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="115"/>
       <c r="D6" s="19" t="s">
         <v>221</v>
       </c>
@@ -17293,8 +17293,8 @@
       <c r="A7" s="98">
         <v>4</v>
       </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="115"/>
       <c r="D7" s="19" t="s">
         <v>222</v>
       </c>
@@ -17315,8 +17315,8 @@
       <c r="A8" s="98">
         <v>5</v>
       </c>
-      <c r="B8" s="111"/>
-      <c r="C8" s="106"/>
+      <c r="B8" s="115"/>
+      <c r="C8" s="103"/>
       <c r="D8" s="19" t="s">
         <v>191</v>
       </c>
@@ -17337,8 +17337,8 @@
       <c r="A9" s="98">
         <v>6</v>
       </c>
-      <c r="B9" s="111"/>
-      <c r="C9" s="126" t="s">
+      <c r="B9" s="115"/>
+      <c r="C9" s="129" t="s">
         <v>223</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -17361,8 +17361,8 @@
       <c r="A10" s="98">
         <v>7</v>
       </c>
-      <c r="B10" s="111"/>
-      <c r="C10" s="111"/>
+      <c r="B10" s="115"/>
+      <c r="C10" s="115"/>
       <c r="D10" s="19" t="s">
         <v>164</v>
       </c>
@@ -17383,8 +17383,8 @@
       <c r="A11" s="98">
         <v>8</v>
       </c>
-      <c r="B11" s="111"/>
-      <c r="C11" s="111"/>
+      <c r="B11" s="115"/>
+      <c r="C11" s="115"/>
       <c r="D11" s="19" t="s">
         <v>224</v>
       </c>
@@ -17405,8 +17405,8 @@
       <c r="A12" s="98">
         <v>9</v>
       </c>
-      <c r="B12" s="111"/>
-      <c r="C12" s="111"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="115"/>
       <c r="D12" s="19" t="s">
         <v>225</v>
       </c>
@@ -17427,8 +17427,8 @@
       <c r="A13" s="98">
         <v>10</v>
       </c>
-      <c r="B13" s="111"/>
-      <c r="C13" s="106"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="103"/>
       <c r="D13" s="19" t="s">
         <v>192</v>
       </c>
@@ -17449,8 +17449,8 @@
       <c r="A14" s="98">
         <v>11</v>
       </c>
-      <c r="B14" s="111"/>
-      <c r="C14" s="126" t="s">
+      <c r="B14" s="115"/>
+      <c r="C14" s="129" t="s">
         <v>226</v>
       </c>
       <c r="D14" s="19" t="s">
@@ -17473,8 +17473,8 @@
       <c r="A15" s="98">
         <v>12</v>
       </c>
-      <c r="B15" s="111"/>
-      <c r="C15" s="111"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="115"/>
       <c r="D15" s="19" t="s">
         <v>165</v>
       </c>
@@ -17495,8 +17495,8 @@
       <c r="A16" s="98">
         <v>13</v>
       </c>
-      <c r="B16" s="111"/>
-      <c r="C16" s="111"/>
+      <c r="B16" s="115"/>
+      <c r="C16" s="115"/>
       <c r="D16" s="19" t="s">
         <v>227</v>
       </c>
@@ -17517,8 +17517,8 @@
       <c r="A17" s="98">
         <v>14</v>
       </c>
-      <c r="B17" s="111"/>
-      <c r="C17" s="111"/>
+      <c r="B17" s="115"/>
+      <c r="C17" s="115"/>
       <c r="D17" s="19" t="s">
         <v>228</v>
       </c>
@@ -17539,8 +17539,8 @@
       <c r="A18" s="98">
         <v>15</v>
       </c>
-      <c r="B18" s="111"/>
-      <c r="C18" s="106"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="103"/>
       <c r="D18" s="19" t="s">
         <v>193</v>
       </c>
@@ -17561,7 +17561,7 @@
       <c r="A19" s="98">
         <v>16</v>
       </c>
-      <c r="B19" s="111"/>
+      <c r="B19" s="115"/>
       <c r="C19" s="19" t="s">
         <v>229</v>
       </c>
@@ -17585,7 +17585,7 @@
       <c r="A20" s="98">
         <v>17</v>
       </c>
-      <c r="B20" s="111"/>
+      <c r="B20" s="115"/>
       <c r="C20" s="19" t="s">
         <v>231</v>
       </c>
@@ -17609,7 +17609,7 @@
       <c r="A21" s="98">
         <v>18</v>
       </c>
-      <c r="B21" s="111"/>
+      <c r="B21" s="115"/>
       <c r="C21" s="19" t="s">
         <v>233</v>
       </c>
@@ -17633,7 +17633,7 @@
       <c r="A22" s="98">
         <v>19</v>
       </c>
-      <c r="B22" s="106"/>
+      <c r="B22" s="103"/>
       <c r="C22" s="19" t="s">
         <v>235</v>
       </c>
@@ -17657,10 +17657,10 @@
       <c r="A23" s="98">
         <v>20</v>
       </c>
-      <c r="B23" s="127" t="s">
+      <c r="B23" s="128" t="s">
         <v>237</v>
       </c>
-      <c r="C23" s="124" t="s">
+      <c r="C23" s="125" t="s">
         <v>220</v>
       </c>
       <c r="D23" s="99" t="s">
@@ -17683,8 +17683,8 @@
       <c r="A24" s="98">
         <v>21</v>
       </c>
-      <c r="B24" s="111"/>
-      <c r="C24" s="111"/>
+      <c r="B24" s="115"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="99" t="s">
         <v>166</v>
       </c>
@@ -17705,8 +17705,8 @@
       <c r="A25" s="98">
         <v>22</v>
       </c>
-      <c r="B25" s="111"/>
-      <c r="C25" s="111"/>
+      <c r="B25" s="115"/>
+      <c r="C25" s="115"/>
       <c r="D25" s="99" t="s">
         <v>238</v>
       </c>
@@ -17727,8 +17727,8 @@
       <c r="A26" s="98">
         <v>23</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
+      <c r="B26" s="115"/>
+      <c r="C26" s="115"/>
       <c r="D26" s="99" t="s">
         <v>239</v>
       </c>
@@ -17749,8 +17749,8 @@
       <c r="A27" s="98">
         <v>24</v>
       </c>
-      <c r="B27" s="111"/>
-      <c r="C27" s="106"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="103"/>
       <c r="D27" s="99" t="s">
         <v>194</v>
       </c>
@@ -17771,8 +17771,8 @@
       <c r="A28" s="98">
         <v>25</v>
       </c>
-      <c r="B28" s="111"/>
-      <c r="C28" s="124" t="s">
+      <c r="B28" s="115"/>
+      <c r="C28" s="125" t="s">
         <v>223</v>
       </c>
       <c r="D28" s="99" t="s">
@@ -17795,8 +17795,8 @@
       <c r="A29" s="98">
         <v>26</v>
       </c>
-      <c r="B29" s="111"/>
-      <c r="C29" s="111"/>
+      <c r="B29" s="115"/>
+      <c r="C29" s="115"/>
       <c r="D29" s="99" t="s">
         <v>167</v>
       </c>
@@ -17817,8 +17817,8 @@
       <c r="A30" s="98">
         <v>27</v>
       </c>
-      <c r="B30" s="111"/>
-      <c r="C30" s="111"/>
+      <c r="B30" s="115"/>
+      <c r="C30" s="115"/>
       <c r="D30" s="99" t="s">
         <v>240</v>
       </c>
@@ -17839,8 +17839,8 @@
       <c r="A31" s="98">
         <v>28</v>
       </c>
-      <c r="B31" s="111"/>
-      <c r="C31" s="111"/>
+      <c r="B31" s="115"/>
+      <c r="C31" s="115"/>
       <c r="D31" s="99" t="s">
         <v>241</v>
       </c>
@@ -17861,8 +17861,8 @@
       <c r="A32" s="98">
         <v>29</v>
       </c>
-      <c r="B32" s="111"/>
-      <c r="C32" s="106"/>
+      <c r="B32" s="115"/>
+      <c r="C32" s="103"/>
       <c r="D32" s="99" t="s">
         <v>195</v>
       </c>
@@ -17883,8 +17883,8 @@
       <c r="A33" s="98">
         <v>30</v>
       </c>
-      <c r="B33" s="111"/>
-      <c r="C33" s="124" t="s">
+      <c r="B33" s="115"/>
+      <c r="C33" s="125" t="s">
         <v>226</v>
       </c>
       <c r="D33" s="99" t="s">
@@ -17907,8 +17907,8 @@
       <c r="A34" s="98">
         <v>31</v>
       </c>
-      <c r="B34" s="111"/>
-      <c r="C34" s="111"/>
+      <c r="B34" s="115"/>
+      <c r="C34" s="115"/>
       <c r="D34" s="99" t="s">
         <v>168</v>
       </c>
@@ -17929,8 +17929,8 @@
       <c r="A35" s="98">
         <v>32</v>
       </c>
-      <c r="B35" s="111"/>
-      <c r="C35" s="111"/>
+      <c r="B35" s="115"/>
+      <c r="C35" s="115"/>
       <c r="D35" s="99" t="s">
         <v>242</v>
       </c>
@@ -17951,8 +17951,8 @@
       <c r="A36" s="98">
         <v>33</v>
       </c>
-      <c r="B36" s="111"/>
-      <c r="C36" s="111"/>
+      <c r="B36" s="115"/>
+      <c r="C36" s="115"/>
       <c r="D36" s="99" t="s">
         <v>243</v>
       </c>
@@ -17973,8 +17973,8 @@
       <c r="A37" s="98">
         <v>34</v>
       </c>
-      <c r="B37" s="111"/>
-      <c r="C37" s="106"/>
+      <c r="B37" s="115"/>
+      <c r="C37" s="103"/>
       <c r="D37" s="99" t="s">
         <v>196</v>
       </c>
@@ -17995,7 +17995,7 @@
       <c r="A38" s="98">
         <v>35</v>
       </c>
-      <c r="B38" s="111"/>
+      <c r="B38" s="115"/>
       <c r="C38" s="99" t="s">
         <v>229</v>
       </c>
@@ -18019,7 +18019,7 @@
       <c r="A39" s="98">
         <v>36</v>
       </c>
-      <c r="B39" s="111"/>
+      <c r="B39" s="115"/>
       <c r="C39" s="99" t="s">
         <v>231</v>
       </c>
@@ -18043,7 +18043,7 @@
       <c r="A40" s="98">
         <v>37</v>
       </c>
-      <c r="B40" s="111"/>
+      <c r="B40" s="115"/>
       <c r="C40" s="99" t="s">
         <v>233</v>
       </c>
@@ -18067,7 +18067,7 @@
       <c r="A41" s="98">
         <v>38</v>
       </c>
-      <c r="B41" s="106"/>
+      <c r="B41" s="103"/>
       <c r="C41" s="99" t="s">
         <v>247</v>
       </c>
@@ -18091,10 +18091,10 @@
       <c r="A42" s="98">
         <v>39</v>
       </c>
-      <c r="B42" s="127" t="s">
+      <c r="B42" s="128" t="s">
         <v>249</v>
       </c>
-      <c r="C42" s="124" t="s">
+      <c r="C42" s="125" t="s">
         <v>220</v>
       </c>
       <c r="D42" s="19" t="s">
@@ -18117,8 +18117,8 @@
       <c r="A43" s="98">
         <v>40</v>
       </c>
-      <c r="B43" s="111"/>
-      <c r="C43" s="111"/>
+      <c r="B43" s="115"/>
+      <c r="C43" s="115"/>
       <c r="D43" s="19" t="s">
         <v>169</v>
       </c>
@@ -18139,8 +18139,8 @@
       <c r="A44" s="98">
         <v>41</v>
       </c>
-      <c r="B44" s="111"/>
-      <c r="C44" s="111"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="115"/>
       <c r="D44" s="19" t="s">
         <v>250</v>
       </c>
@@ -18161,8 +18161,8 @@
       <c r="A45" s="98">
         <v>42</v>
       </c>
-      <c r="B45" s="111"/>
-      <c r="C45" s="111"/>
+      <c r="B45" s="115"/>
+      <c r="C45" s="115"/>
       <c r="D45" s="19" t="s">
         <v>251</v>
       </c>
@@ -18183,8 +18183,8 @@
       <c r="A46" s="98">
         <v>43</v>
       </c>
-      <c r="B46" s="111"/>
-      <c r="C46" s="106"/>
+      <c r="B46" s="115"/>
+      <c r="C46" s="103"/>
       <c r="D46" s="19" t="s">
         <v>197</v>
       </c>
@@ -18205,8 +18205,8 @@
       <c r="A47" s="98">
         <v>44</v>
       </c>
-      <c r="B47" s="111"/>
-      <c r="C47" s="124" t="s">
+      <c r="B47" s="115"/>
+      <c r="C47" s="125" t="s">
         <v>223</v>
       </c>
       <c r="D47" s="19" t="s">
@@ -18229,8 +18229,8 @@
       <c r="A48" s="98">
         <v>45</v>
       </c>
-      <c r="B48" s="111"/>
-      <c r="C48" s="111"/>
+      <c r="B48" s="115"/>
+      <c r="C48" s="115"/>
       <c r="D48" s="19" t="s">
         <v>170</v>
       </c>
@@ -18251,8 +18251,8 @@
       <c r="A49" s="98">
         <v>46</v>
       </c>
-      <c r="B49" s="111"/>
-      <c r="C49" s="111"/>
+      <c r="B49" s="115"/>
+      <c r="C49" s="115"/>
       <c r="D49" s="19" t="s">
         <v>252</v>
       </c>
@@ -18273,8 +18273,8 @@
       <c r="A50" s="98">
         <v>47</v>
       </c>
-      <c r="B50" s="111"/>
-      <c r="C50" s="111"/>
+      <c r="B50" s="115"/>
+      <c r="C50" s="115"/>
       <c r="D50" s="19" t="s">
         <v>253</v>
       </c>
@@ -18295,8 +18295,8 @@
       <c r="A51" s="98">
         <v>48</v>
       </c>
-      <c r="B51" s="111"/>
-      <c r="C51" s="106"/>
+      <c r="B51" s="115"/>
+      <c r="C51" s="103"/>
       <c r="D51" s="19" t="s">
         <v>198</v>
       </c>
@@ -18317,8 +18317,8 @@
       <c r="A52" s="98">
         <v>49</v>
       </c>
-      <c r="B52" s="111"/>
-      <c r="C52" s="124" t="s">
+      <c r="B52" s="115"/>
+      <c r="C52" s="125" t="s">
         <v>226</v>
       </c>
       <c r="D52" s="19" t="s">
@@ -18341,8 +18341,8 @@
       <c r="A53" s="98">
         <v>50</v>
       </c>
-      <c r="B53" s="111"/>
-      <c r="C53" s="111"/>
+      <c r="B53" s="115"/>
+      <c r="C53" s="115"/>
       <c r="D53" s="19" t="s">
         <v>171</v>
       </c>
@@ -18363,8 +18363,8 @@
       <c r="A54" s="98">
         <v>51</v>
       </c>
-      <c r="B54" s="111"/>
-      <c r="C54" s="111"/>
+      <c r="B54" s="115"/>
+      <c r="C54" s="115"/>
       <c r="D54" s="19" t="s">
         <v>254</v>
       </c>
@@ -18385,8 +18385,8 @@
       <c r="A55" s="98">
         <v>52</v>
       </c>
-      <c r="B55" s="111"/>
-      <c r="C55" s="111"/>
+      <c r="B55" s="115"/>
+      <c r="C55" s="115"/>
       <c r="D55" s="19" t="s">
         <v>255</v>
       </c>
@@ -18407,8 +18407,8 @@
       <c r="A56" s="98">
         <v>53</v>
       </c>
-      <c r="B56" s="111"/>
-      <c r="C56" s="106"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="103"/>
       <c r="D56" s="19" t="s">
         <v>199</v>
       </c>
@@ -18429,7 +18429,7 @@
       <c r="A57" s="98">
         <v>54</v>
       </c>
-      <c r="B57" s="111"/>
+      <c r="B57" s="115"/>
       <c r="C57" s="99" t="s">
         <v>229</v>
       </c>
@@ -18453,7 +18453,7 @@
       <c r="A58" s="98">
         <v>55</v>
       </c>
-      <c r="B58" s="111"/>
+      <c r="B58" s="115"/>
       <c r="C58" s="99" t="s">
         <v>231</v>
       </c>
@@ -18477,7 +18477,7 @@
       <c r="A59" s="98">
         <v>56</v>
       </c>
-      <c r="B59" s="111"/>
+      <c r="B59" s="115"/>
       <c r="C59" s="99" t="s">
         <v>233</v>
       </c>
@@ -18501,7 +18501,7 @@
       <c r="A60" s="98">
         <v>57</v>
       </c>
-      <c r="B60" s="106"/>
+      <c r="B60" s="103"/>
       <c r="C60" s="99" t="s">
         <v>235</v>
       </c>
@@ -18525,10 +18525,10 @@
       <c r="A61" s="98">
         <v>58</v>
       </c>
-      <c r="B61" s="129" t="s">
+      <c r="B61" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="C61" s="124" t="s">
+      <c r="C61" s="125" t="s">
         <v>220</v>
       </c>
       <c r="D61" s="19" t="s">
@@ -18551,8 +18551,8 @@
       <c r="A62" s="98">
         <v>59</v>
       </c>
-      <c r="B62" s="111"/>
-      <c r="C62" s="111"/>
+      <c r="B62" s="115"/>
+      <c r="C62" s="115"/>
       <c r="D62" s="19" t="s">
         <v>160</v>
       </c>
@@ -18573,8 +18573,8 @@
       <c r="A63" s="98">
         <v>60</v>
       </c>
-      <c r="B63" s="111"/>
-      <c r="C63" s="111"/>
+      <c r="B63" s="115"/>
+      <c r="C63" s="115"/>
       <c r="D63" s="19" t="s">
         <v>261</v>
       </c>
@@ -18595,8 +18595,8 @@
       <c r="A64" s="98">
         <v>61</v>
       </c>
-      <c r="B64" s="111"/>
-      <c r="C64" s="111"/>
+      <c r="B64" s="115"/>
+      <c r="C64" s="115"/>
       <c r="D64" s="19" t="s">
         <v>262</v>
       </c>
@@ -18617,8 +18617,8 @@
       <c r="A65" s="98">
         <v>62</v>
       </c>
-      <c r="B65" s="111"/>
-      <c r="C65" s="106"/>
+      <c r="B65" s="115"/>
+      <c r="C65" s="103"/>
       <c r="D65" s="19" t="s">
         <v>188</v>
       </c>
@@ -18639,8 +18639,8 @@
       <c r="A66" s="98">
         <v>63</v>
       </c>
-      <c r="B66" s="111"/>
-      <c r="C66" s="124" t="s">
+      <c r="B66" s="115"/>
+      <c r="C66" s="125" t="s">
         <v>223</v>
       </c>
       <c r="D66" s="19" t="s">
@@ -18663,8 +18663,8 @@
       <c r="A67" s="98">
         <v>64</v>
       </c>
-      <c r="B67" s="111"/>
-      <c r="C67" s="111"/>
+      <c r="B67" s="115"/>
+      <c r="C67" s="115"/>
       <c r="D67" s="19" t="s">
         <v>161</v>
       </c>
@@ -18685,8 +18685,8 @@
       <c r="A68" s="98">
         <v>65</v>
       </c>
-      <c r="B68" s="111"/>
-      <c r="C68" s="111"/>
+      <c r="B68" s="115"/>
+      <c r="C68" s="115"/>
       <c r="D68" s="19" t="s">
         <v>263</v>
       </c>
@@ -18707,8 +18707,8 @@
       <c r="A69" s="98">
         <v>66</v>
       </c>
-      <c r="B69" s="111"/>
-      <c r="C69" s="111"/>
+      <c r="B69" s="115"/>
+      <c r="C69" s="115"/>
       <c r="D69" s="19" t="s">
         <v>264</v>
       </c>
@@ -18729,8 +18729,8 @@
       <c r="A70" s="98">
         <v>67</v>
       </c>
-      <c r="B70" s="111"/>
-      <c r="C70" s="106"/>
+      <c r="B70" s="115"/>
+      <c r="C70" s="103"/>
       <c r="D70" s="19" t="s">
         <v>189</v>
       </c>
@@ -18751,8 +18751,8 @@
       <c r="A71" s="98">
         <v>68</v>
       </c>
-      <c r="B71" s="111"/>
-      <c r="C71" s="124" t="s">
+      <c r="B71" s="115"/>
+      <c r="C71" s="125" t="s">
         <v>226</v>
       </c>
       <c r="D71" s="19" t="s">
@@ -18775,8 +18775,8 @@
       <c r="A72" s="98">
         <v>69</v>
       </c>
-      <c r="B72" s="111"/>
-      <c r="C72" s="111"/>
+      <c r="B72" s="115"/>
+      <c r="C72" s="115"/>
       <c r="D72" s="19" t="s">
         <v>162</v>
       </c>
@@ -18797,8 +18797,8 @@
       <c r="A73" s="98">
         <v>70</v>
       </c>
-      <c r="B73" s="111"/>
-      <c r="C73" s="111"/>
+      <c r="B73" s="115"/>
+      <c r="C73" s="115"/>
       <c r="D73" s="19" t="s">
         <v>265</v>
       </c>
@@ -18819,8 +18819,8 @@
       <c r="A74" s="98">
         <v>71</v>
       </c>
-      <c r="B74" s="111"/>
-      <c r="C74" s="111"/>
+      <c r="B74" s="115"/>
+      <c r="C74" s="115"/>
       <c r="D74" s="19" t="s">
         <v>266</v>
       </c>
@@ -18841,8 +18841,8 @@
       <c r="A75" s="98">
         <v>72</v>
       </c>
-      <c r="B75" s="111"/>
-      <c r="C75" s="106"/>
+      <c r="B75" s="115"/>
+      <c r="C75" s="103"/>
       <c r="D75" s="19" t="s">
         <v>190</v>
       </c>
@@ -18863,7 +18863,7 @@
       <c r="A76" s="98">
         <v>73</v>
       </c>
-      <c r="B76" s="111"/>
+      <c r="B76" s="115"/>
       <c r="C76" s="99" t="s">
         <v>229</v>
       </c>
@@ -18887,7 +18887,7 @@
       <c r="A77" s="98">
         <v>74</v>
       </c>
-      <c r="B77" s="111"/>
+      <c r="B77" s="115"/>
       <c r="C77" s="99" t="s">
         <v>231</v>
       </c>
@@ -18911,7 +18911,7 @@
       <c r="A78" s="98">
         <v>75</v>
       </c>
-      <c r="B78" s="111"/>
+      <c r="B78" s="115"/>
       <c r="C78" s="99" t="s">
         <v>233</v>
       </c>
@@ -18935,7 +18935,7 @@
       <c r="A79" s="98">
         <v>76</v>
       </c>
-      <c r="B79" s="106"/>
+      <c r="B79" s="103"/>
       <c r="C79" s="99" t="s">
         <v>235</v>
       </c>
@@ -18959,10 +18959,10 @@
       <c r="A80" s="98">
         <v>77</v>
       </c>
-      <c r="B80" s="125" t="s">
+      <c r="B80" s="131" t="s">
         <v>271</v>
       </c>
-      <c r="C80" s="124" t="s">
+      <c r="C80" s="125" t="s">
         <v>130</v>
       </c>
       <c r="D80" s="19" t="s">
@@ -18985,8 +18985,8 @@
       <c r="A81" s="98">
         <v>78</v>
       </c>
-      <c r="B81" s="111"/>
-      <c r="C81" s="111"/>
+      <c r="B81" s="115"/>
+      <c r="C81" s="115"/>
       <c r="D81" s="19" t="s">
         <v>157</v>
       </c>
@@ -19007,8 +19007,8 @@
       <c r="A82" s="98">
         <v>79</v>
       </c>
-      <c r="B82" s="111"/>
-      <c r="C82" s="111"/>
+      <c r="B82" s="115"/>
+      <c r="C82" s="115"/>
       <c r="D82" s="19" t="s">
         <v>272</v>
       </c>
@@ -19029,8 +19029,8 @@
       <c r="A83" s="98">
         <v>80</v>
       </c>
-      <c r="B83" s="111"/>
-      <c r="C83" s="111"/>
+      <c r="B83" s="115"/>
+      <c r="C83" s="115"/>
       <c r="D83" s="19" t="s">
         <v>273</v>
       </c>
@@ -19051,8 +19051,8 @@
       <c r="A84" s="98">
         <v>81</v>
       </c>
-      <c r="B84" s="111"/>
-      <c r="C84" s="106"/>
+      <c r="B84" s="115"/>
+      <c r="C84" s="103"/>
       <c r="D84" s="19" t="s">
         <v>186</v>
       </c>
@@ -19073,8 +19073,8 @@
       <c r="A85" s="98">
         <v>82</v>
       </c>
-      <c r="B85" s="111"/>
-      <c r="C85" s="124" t="s">
+      <c r="B85" s="115"/>
+      <c r="C85" s="125" t="s">
         <v>133</v>
       </c>
       <c r="D85" s="19" t="s">
@@ -19097,8 +19097,8 @@
       <c r="A86" s="98">
         <v>83</v>
       </c>
-      <c r="B86" s="111"/>
-      <c r="C86" s="111"/>
+      <c r="B86" s="115"/>
+      <c r="C86" s="115"/>
       <c r="D86" s="19" t="s">
         <v>159</v>
       </c>
@@ -19119,8 +19119,8 @@
       <c r="A87" s="98">
         <v>84</v>
       </c>
-      <c r="B87" s="111"/>
-      <c r="C87" s="111"/>
+      <c r="B87" s="115"/>
+      <c r="C87" s="115"/>
       <c r="D87" s="19" t="s">
         <v>274</v>
       </c>
@@ -19141,8 +19141,8 @@
       <c r="A88" s="98">
         <v>85</v>
       </c>
-      <c r="B88" s="111"/>
-      <c r="C88" s="111"/>
+      <c r="B88" s="115"/>
+      <c r="C88" s="115"/>
       <c r="D88" s="19" t="s">
         <v>275</v>
       </c>
@@ -19163,8 +19163,8 @@
       <c r="A89" s="98">
         <v>86</v>
       </c>
-      <c r="B89" s="111"/>
-      <c r="C89" s="106"/>
+      <c r="B89" s="115"/>
+      <c r="C89" s="103"/>
       <c r="D89" s="19" t="s">
         <v>187</v>
       </c>
@@ -19185,8 +19185,8 @@
       <c r="A90" s="98">
         <v>87</v>
       </c>
-      <c r="B90" s="111"/>
-      <c r="C90" s="124" t="s">
+      <c r="B90" s="115"/>
+      <c r="C90" s="125" t="s">
         <v>276</v>
       </c>
       <c r="D90" s="19" t="s">
@@ -19209,8 +19209,8 @@
       <c r="A91" s="98">
         <v>88</v>
       </c>
-      <c r="B91" s="111"/>
-      <c r="C91" s="111"/>
+      <c r="B91" s="115"/>
+      <c r="C91" s="115"/>
       <c r="D91" s="19" t="s">
         <v>278</v>
       </c>
@@ -19231,8 +19231,8 @@
       <c r="A92" s="98">
         <v>89</v>
       </c>
-      <c r="B92" s="111"/>
-      <c r="C92" s="111"/>
+      <c r="B92" s="115"/>
+      <c r="C92" s="115"/>
       <c r="D92" s="19" t="s">
         <v>279</v>
       </c>
@@ -19253,8 +19253,8 @@
       <c r="A93" s="98">
         <v>90</v>
       </c>
-      <c r="B93" s="111"/>
-      <c r="C93" s="111"/>
+      <c r="B93" s="115"/>
+      <c r="C93" s="115"/>
       <c r="D93" s="19" t="s">
         <v>280</v>
       </c>
@@ -19275,8 +19275,8 @@
       <c r="A94" s="98">
         <v>91</v>
       </c>
-      <c r="B94" s="111"/>
-      <c r="C94" s="106"/>
+      <c r="B94" s="115"/>
+      <c r="C94" s="103"/>
       <c r="D94" s="19" t="s">
         <v>281</v>
       </c>
@@ -19297,8 +19297,8 @@
       <c r="A95" s="98">
         <v>92</v>
       </c>
-      <c r="B95" s="111"/>
-      <c r="C95" s="124" t="s">
+      <c r="B95" s="115"/>
+      <c r="C95" s="125" t="s">
         <v>282</v>
       </c>
       <c r="D95" s="19" t="s">
@@ -19321,8 +19321,8 @@
       <c r="A96" s="98">
         <v>93</v>
       </c>
-      <c r="B96" s="111"/>
-      <c r="C96" s="111"/>
+      <c r="B96" s="115"/>
+      <c r="C96" s="115"/>
       <c r="D96" s="19" t="s">
         <v>284</v>
       </c>
@@ -19343,8 +19343,8 @@
       <c r="A97" s="98">
         <v>94</v>
       </c>
-      <c r="B97" s="111"/>
-      <c r="C97" s="111"/>
+      <c r="B97" s="115"/>
+      <c r="C97" s="115"/>
       <c r="D97" s="19" t="s">
         <v>285</v>
       </c>
@@ -19365,8 +19365,8 @@
       <c r="A98" s="98">
         <v>95</v>
       </c>
-      <c r="B98" s="111"/>
-      <c r="C98" s="111"/>
+      <c r="B98" s="115"/>
+      <c r="C98" s="115"/>
       <c r="D98" s="19" t="s">
         <v>286</v>
       </c>
@@ -19387,8 +19387,8 @@
       <c r="A99" s="98">
         <v>96</v>
       </c>
-      <c r="B99" s="111"/>
-      <c r="C99" s="106"/>
+      <c r="B99" s="115"/>
+      <c r="C99" s="103"/>
       <c r="D99" s="19" t="s">
         <v>287</v>
       </c>
@@ -19409,8 +19409,8 @@
       <c r="A100" s="98">
         <v>97</v>
       </c>
-      <c r="B100" s="111"/>
-      <c r="C100" s="124" t="s">
+      <c r="B100" s="115"/>
+      <c r="C100" s="125" t="s">
         <v>288</v>
       </c>
       <c r="D100" s="19" t="s">
@@ -19433,8 +19433,8 @@
       <c r="A101" s="98">
         <v>98</v>
       </c>
-      <c r="B101" s="111"/>
-      <c r="C101" s="111"/>
+      <c r="B101" s="115"/>
+      <c r="C101" s="115"/>
       <c r="D101" s="19" t="s">
         <v>290</v>
       </c>
@@ -19455,8 +19455,8 @@
       <c r="A102" s="98">
         <v>99</v>
       </c>
-      <c r="B102" s="111"/>
-      <c r="C102" s="111"/>
+      <c r="B102" s="115"/>
+      <c r="C102" s="115"/>
       <c r="D102" s="19" t="s">
         <v>291</v>
       </c>
@@ -19477,8 +19477,8 @@
       <c r="A103" s="98">
         <v>100</v>
       </c>
-      <c r="B103" s="111"/>
-      <c r="C103" s="111"/>
+      <c r="B103" s="115"/>
+      <c r="C103" s="115"/>
       <c r="D103" s="19" t="s">
         <v>292</v>
       </c>
@@ -19499,8 +19499,8 @@
       <c r="A104" s="98">
         <v>101</v>
       </c>
-      <c r="B104" s="111"/>
-      <c r="C104" s="106"/>
+      <c r="B104" s="115"/>
+      <c r="C104" s="103"/>
       <c r="D104" s="19" t="s">
         <v>293</v>
       </c>
@@ -19521,8 +19521,8 @@
       <c r="A105" s="98">
         <v>102</v>
       </c>
-      <c r="B105" s="111"/>
-      <c r="C105" s="124" t="s">
+      <c r="B105" s="115"/>
+      <c r="C105" s="125" t="s">
         <v>294</v>
       </c>
       <c r="D105" s="19" t="s">
@@ -19545,8 +19545,8 @@
       <c r="A106" s="98">
         <v>103</v>
       </c>
-      <c r="B106" s="111"/>
-      <c r="C106" s="111"/>
+      <c r="B106" s="115"/>
+      <c r="C106" s="115"/>
       <c r="D106" s="19" t="s">
         <v>296</v>
       </c>
@@ -19567,8 +19567,8 @@
       <c r="A107" s="98">
         <v>104</v>
       </c>
-      <c r="B107" s="111"/>
-      <c r="C107" s="111"/>
+      <c r="B107" s="115"/>
+      <c r="C107" s="115"/>
       <c r="D107" s="19" t="s">
         <v>297</v>
       </c>
@@ -19589,8 +19589,8 @@
       <c r="A108" s="98">
         <v>105</v>
       </c>
-      <c r="B108" s="111"/>
-      <c r="C108" s="111"/>
+      <c r="B108" s="115"/>
+      <c r="C108" s="115"/>
       <c r="D108" s="19" t="s">
         <v>298</v>
       </c>
@@ -19611,8 +19611,8 @@
       <c r="A109" s="98">
         <v>106</v>
       </c>
-      <c r="B109" s="111"/>
-      <c r="C109" s="106"/>
+      <c r="B109" s="115"/>
+      <c r="C109" s="103"/>
       <c r="D109" s="19" t="s">
         <v>299</v>
       </c>
@@ -19633,8 +19633,8 @@
       <c r="A110" s="98">
         <v>107</v>
       </c>
-      <c r="B110" s="111"/>
-      <c r="C110" s="124" t="s">
+      <c r="B110" s="115"/>
+      <c r="C110" s="125" t="s">
         <v>300</v>
       </c>
       <c r="D110" s="19" t="s">
@@ -19657,8 +19657,8 @@
       <c r="A111" s="98">
         <v>108</v>
       </c>
-      <c r="B111" s="111"/>
-      <c r="C111" s="111"/>
+      <c r="B111" s="115"/>
+      <c r="C111" s="115"/>
       <c r="D111" s="19" t="s">
         <v>302</v>
       </c>
@@ -19679,8 +19679,8 @@
       <c r="A112" s="98">
         <v>109</v>
       </c>
-      <c r="B112" s="111"/>
-      <c r="C112" s="111"/>
+      <c r="B112" s="115"/>
+      <c r="C112" s="115"/>
       <c r="D112" s="19" t="s">
         <v>303</v>
       </c>
@@ -19701,8 +19701,8 @@
       <c r="A113" s="98">
         <v>110</v>
       </c>
-      <c r="B113" s="111"/>
-      <c r="C113" s="111"/>
+      <c r="B113" s="115"/>
+      <c r="C113" s="115"/>
       <c r="D113" s="19" t="s">
         <v>304</v>
       </c>
@@ -19723,8 +19723,8 @@
       <c r="A114" s="98">
         <v>111</v>
       </c>
-      <c r="B114" s="111"/>
-      <c r="C114" s="106"/>
+      <c r="B114" s="115"/>
+      <c r="C114" s="103"/>
       <c r="D114" s="19" t="s">
         <v>305</v>
       </c>
@@ -19745,8 +19745,8 @@
       <c r="A115" s="98">
         <v>112</v>
       </c>
-      <c r="B115" s="111"/>
-      <c r="C115" s="124" t="s">
+      <c r="B115" s="115"/>
+      <c r="C115" s="125" t="s">
         <v>306</v>
       </c>
       <c r="D115" s="19" t="s">
@@ -19769,8 +19769,8 @@
       <c r="A116" s="98">
         <v>113</v>
       </c>
-      <c r="B116" s="111"/>
-      <c r="C116" s="111"/>
+      <c r="B116" s="115"/>
+      <c r="C116" s="115"/>
       <c r="D116" s="19" t="s">
         <v>308</v>
       </c>
@@ -19791,8 +19791,8 @@
       <c r="A117" s="98">
         <v>114</v>
       </c>
-      <c r="B117" s="111"/>
-      <c r="C117" s="111"/>
+      <c r="B117" s="115"/>
+      <c r="C117" s="115"/>
       <c r="D117" s="19" t="s">
         <v>309</v>
       </c>
@@ -19813,8 +19813,8 @@
       <c r="A118" s="98">
         <v>115</v>
       </c>
-      <c r="B118" s="111"/>
-      <c r="C118" s="111"/>
+      <c r="B118" s="115"/>
+      <c r="C118" s="115"/>
       <c r="D118" s="19" t="s">
         <v>310</v>
       </c>
@@ -19835,8 +19835,8 @@
       <c r="A119" s="98">
         <v>116</v>
       </c>
-      <c r="B119" s="106"/>
-      <c r="C119" s="106"/>
+      <c r="B119" s="103"/>
+      <c r="C119" s="103"/>
       <c r="D119" s="19" t="s">
         <v>311</v>
       </c>
@@ -22498,21 +22498,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B61:B79"/>
-    <mergeCell ref="C61:C65"/>
-    <mergeCell ref="C66:C70"/>
-    <mergeCell ref="C71:C75"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="C47:C51"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B4:B22"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="B42:B60"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="C80:C84"/>
     <mergeCell ref="C85:C89"/>
     <mergeCell ref="B80:B119"/>
@@ -22529,6 +22514,21 @@
     <mergeCell ref="C105:C109"/>
     <mergeCell ref="C110:C114"/>
     <mergeCell ref="C115:C119"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B4:B22"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="B42:B60"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B61:B79"/>
+    <mergeCell ref="C61:C65"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="C71:C75"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="C47:C51"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:G119">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">

</xml_diff>